<commit_message>
Add reviewers and "dated" warning in workbook.
</commit_message>
<xml_diff>
--- a/src/Planning/understand-options-tfs-vsts-environments-capacity-guide.xlsx
+++ b/src/Planning/understand-options-tfs-vsts-environments-capacity-guide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willy\OneDrive\_sandbox\planning guide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willy\OneDrive\_repos\Guidance\src\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_481838BC9F82B1C870C8F03207606A56245E0862" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{B660518E-83CE-48D7-B6B4-7AF39787574A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0122CD-E99A-4E71-A639-93191298AE4B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="7812" windowWidth="21840" windowHeight="7272" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12" yWindow="8268" windowWidth="21840" windowHeight="7272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server Scenarios" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
     <definedName name="STANDARD_USERS">Constants!$C$3</definedName>
     <definedName name="VIRTUAL_PERCENTAGE">Constants!$B$19</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -352,9 +352,6 @@
     <t>DISK-DT</t>
   </si>
   <si>
-    <t>Review the Real-World “Beef” Factor section in the TFS Project Guidance document.</t>
-  </si>
-  <si>
     <t>BETA</t>
   </si>
   <si>
@@ -411,9 +408,6 @@
       </rPr>
       <t xml:space="preserve"> FACTOR</t>
     </r>
-  </si>
-  <si>
-    <t>Version 2012.02.24</t>
   </si>
   <si>
     <r>
@@ -450,6 +444,12 @@
       </rPr>
       <t>This is a simplified model for educational purposes and does not replace expert consulting. Real-world requirements and infrastructure environments can be much more complex.</t>
     </r>
+  </si>
+  <si>
+    <t>Version 2012.02.24 (DATED!)</t>
+  </si>
+  <si>
+    <t>Safety growth factor to add to proposed arcjitecture.</t>
   </si>
 </sst>
 </file>
@@ -1145,6 +1145,66 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1163,108 +1223,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1284,6 +1242,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1732,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1758,56 +1758,56 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="74" t="s">
+      <c r="A5" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="75"/>
+      <c r="C5" s="95"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="1.65">
-      <c r="A6" s="70"/>
+      <c r="A6" s="90"/>
       <c r="B6" s="66" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="67">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>1</v>
       </c>
       <c r="I6" s="64" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="71"/>
+      <c r="A7" s="91"/>
       <c r="B7" s="68" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="69">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>3</v>
@@ -1828,7 +1828,7 @@
         <v>0.25</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1838,111 +1838,111 @@
       <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76" t="s">
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76" t="s">
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="76"/>
-      <c r="K11" s="94"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="83"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="73"/>
-      <c r="C12" s="77" t="s">
+      <c r="B12" s="93"/>
+      <c r="C12" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77" t="s">
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77" t="s">
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="77"/>
-      <c r="K12" s="95"/>
+      <c r="J12" s="84"/>
+      <c r="K12" s="85"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="80" t="str">
+      <c r="C13" s="86" t="str">
         <f>IF(Current_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80" t="str">
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86" t="str">
         <f>IF(Current_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80" t="str">
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86" t="str">
         <f>I14</f>
-        <v>Yes</v>
-      </c>
-      <c r="J13" s="80"/>
-      <c r="K13" s="83"/>
+        <v>No</v>
+      </c>
+      <c r="J13" s="86"/>
+      <c r="K13" s="87"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="81" t="str">
+      <c r="C14" s="88" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
-        <v>No</v>
-      </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88" t="str">
         <f>IF(Future_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81" t="str">
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_YES,C_NO)</f>
-        <v>Yes</v>
-      </c>
-      <c r="J14" s="81"/>
-      <c r="K14" s="84"/>
+        <v>No</v>
+      </c>
+      <c r="J14" s="88"/>
+      <c r="K14" s="89"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="81" t="str">
+      <c r="C15" s="88" t="str">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;1),C_YES,C_NO)</f>
-        <v>No</v>
-      </c>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;1),C_YES,C_NO)</f>
         <v>Yes</v>
       </c>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="81" t="str">
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88" t="str">
         <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),C_YES,C_NO)</f>
-        <v>Yes</v>
-      </c>
-      <c r="J15" s="81"/>
-      <c r="K15" s="84"/>
+        <v>No</v>
+      </c>
+      <c r="J15" s="88"/>
+      <c r="K15" s="89"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="28" t="s">
@@ -1954,47 +1954,47 @@
       </c>
       <c r="D16" s="30" t="str">
         <f>IF(E16="","","-")</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E16" s="31" t="str">
         <f>IF(C14=C_YES,(IF(Future_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
-        <v/>
-      </c>
-      <c r="F16" s="82" t="str">
+        <v>Low-End</v>
+      </c>
+      <c r="F16" s="71" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),"High-End","")</f>
         <v>High-End</v>
       </c>
-      <c r="G16" s="82"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="82" t="str">
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),"Scale Unit","")</f>
         <v>Scale Unit</v>
       </c>
-      <c r="J16" s="82"/>
-      <c r="K16" s="86"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="72"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="78">
+      <c r="C17" s="73">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
         <v>5</v>
       </c>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78">
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73">
         <f>IF(F13=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78">
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73" t="str">
         <f>IF(I13=C_YES,SCALE_TPC,"")</f>
-        <v>75</v>
-      </c>
-      <c r="J17" s="78"/>
-      <c r="K17" s="91"/>
+        <v/>
+      </c>
+      <c r="J17" s="73"/>
+      <c r="K17" s="78"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="33" t="s">
@@ -2002,114 +2002,114 @@
       </c>
       <c r="C18" s="79">
         <f>IF(C13=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D18" s="79"/>
       <c r="E18" s="79"/>
-      <c r="F18" s="78">
+      <c r="F18" s="73">
         <f>IF(F14=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="79">
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="79" t="str">
         <f>IF(I14=C_YES,SCALE_TPC,"")</f>
-        <v>75</v>
+        <v/>
       </c>
       <c r="J18" s="79"/>
-      <c r="K18" s="92"/>
+      <c r="K18" s="80"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="93">
+      <c r="C19" s="81">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93">
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="G19" s="93"/>
-      <c r="H19" s="93"/>
-      <c r="I19" s="34">
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="34" t="str">
         <f>IF(I13=C_YES,ROUNDUP(I20/SCALE_RPS,0),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="J19" s="35" t="str">
         <f>IF(K19&lt;&gt;"","-","")</f>
-        <v>-</v>
-      </c>
-      <c r="K19" s="36">
+        <v/>
+      </c>
+      <c r="K19" s="36" t="str">
         <f>IF(I14=C_YES,ROUNDUP(K20/SCALE_RPS,0),"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="87">
+      <c r="C20" s="74">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,Current_Users*STANDARD_FACTOR,Current_Users*LO_FACTOR)),"")</f>
-        <v>35</v>
-      </c>
-      <c r="D20" s="87" t="str">
+        <v>0</v>
+      </c>
+      <c r="D20" s="74" t="str">
         <f>IF(E20&lt;&gt;"","-","")</f>
-        <v/>
-      </c>
-      <c r="E20" s="87" t="str">
+        <v>-</v>
+      </c>
+      <c r="E20" s="74">
         <f>IF(C14=C_YES,(IF(Future_Users&gt;LO_USERS,Future_Users*STANDARD_FACTOR,Future_Users*LO_FACTOR)),"")</f>
-        <v/>
-      </c>
-      <c r="F20" s="89">
+        <v>0</v>
+      </c>
+      <c r="F20" s="76">
         <f>IF(F13=C_YES,Current_Users*HI_FACTOR,"")</f>
-        <v>45</v>
-      </c>
-      <c r="G20" s="87" t="str">
+        <v>0</v>
+      </c>
+      <c r="G20" s="74" t="str">
         <f>IF(H20&lt;&gt;"","-","")</f>
         <v>-</v>
       </c>
-      <c r="H20" s="89">
+      <c r="H20" s="76">
         <f>IF(F14=C_YES,Future_Users*HI_FACTOR,"")</f>
-        <v>450</v>
-      </c>
-      <c r="I20" s="37">
+        <v>0</v>
+      </c>
+      <c r="I20" s="37" t="str">
         <f>IF(I13=C_YES,Current_Users*SCALE_FACTOR,"")</f>
-        <v>52.5</v>
+        <v/>
       </c>
       <c r="J20" s="38" t="str">
         <f>IF(K20&lt;&gt;"","-","")</f>
-        <v>-</v>
-      </c>
-      <c r="K20" s="39">
+        <v/>
+      </c>
+      <c r="K20" s="39" t="str">
         <f>IF(I13=C_YES,Future_Users*HI_FACTOR,"")</f>
-        <v>450</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="88"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="41">
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="41" t="str">
         <f>IF(I13=C_YES,I20/I19,"")</f>
-        <v>52.5</v>
+        <v/>
       </c>
       <c r="J21" s="42" t="str">
         <f>IF(K21&lt;&gt;"","-","")</f>
-        <v>-</v>
-      </c>
-      <c r="K21" s="43">
+        <v/>
+      </c>
+      <c r="K21" s="43" t="str">
         <f>IF(I14=C_YES,K20/K19,"")</f>
-        <v>450</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="2:11" ht="91.8" x14ac:dyDescent="1.65">
@@ -2117,6 +2117,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="F17:H17"/>
@@ -2133,25 +2152,6 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="I12:K12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
     <cfRule type="expression" dxfId="7" priority="13">
@@ -2215,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2233,21 +2233,21 @@
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="116" t="str">
+      <c r="B2" s="102" t="str">
         <f>'Server Scenarios'!B2:K2</f>
-        <v>Version 2012.02.24</v>
-      </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
+        <v>Version 2012.02.24 (DATED!)</v>
+      </c>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -2256,31 +2256,31 @@
     </row>
     <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="110" t="s">
-        <v>55</v>
+      <c r="B5" s="96" t="s">
+        <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="96" t="s">
+      <c r="D5" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="97"/>
-      <c r="F5" s="96" t="s">
+      <c r="E5" s="111"/>
+      <c r="F5" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="96" t="s">
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="97"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="111"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="111"/>
+      <c r="B6" s="97"/>
       <c r="C6" s="3"/>
       <c r="D6" s="14" t="s">
         <v>13</v>
@@ -2288,25 +2288,25 @@
       <c r="E6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="99" t="s">
+      <c r="F6" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="100"/>
-      <c r="H6" s="101" t="s">
+      <c r="G6" s="114"/>
+      <c r="H6" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="100"/>
-      <c r="J6" s="99" t="s">
+      <c r="I6" s="114"/>
+      <c r="J6" s="113" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101" t="s">
+      <c r="K6" s="114"/>
+      <c r="L6" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="M6" s="102"/>
+      <c r="M6" s="116"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="111"/>
+      <c r="B7" s="97"/>
       <c r="C7" s="3"/>
       <c r="D7" s="14" t="s">
         <v>8</v>
@@ -2340,7 +2340,7 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="111"/>
+      <c r="B8" s="97"/>
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
@@ -2370,23 +2370,23 @@
       </c>
       <c r="J8" s="48">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_CORE_AT,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8" s="51">
         <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_CORE_DT,HI_CORE_DT)),0)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L8" s="52">
         <f>J8+J8*VIRTUAL_PERCENTAGE</f>
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="M8" s="53">
         <f>IF(K8&lt;&gt;"",ROUNDUP(K8+K8*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="111"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="4" t="s">
         <v>18</v>
       </c>
@@ -2416,23 +2416,23 @@
       </c>
       <c r="J9" s="48">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_RAM_AT,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K9" s="51">
         <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_RAM_DT,HI_RAM_DT)),0)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L9" s="52">
         <f>J9+J9*VIRTUAL_PERCENTAGE</f>
-        <v>4.8</v>
+        <v>0</v>
       </c>
       <c r="M9" s="53">
         <f>IF(K9&lt;&gt;"",ROUNDUP(K9+K9*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="111"/>
+      <c r="B10" s="97"/>
       <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
@@ -2462,23 +2462,23 @@
       </c>
       <c r="J10" s="49">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_DISK_AT,0)</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="K10" s="54">
         <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_DISK_DT,HI_DISK_DT)),0)</f>
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="L10" s="63">
         <f>J10+J10*VIRTUAL_PERCENTAGE</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="M10" s="55">
         <f>IF(K10&lt;&gt;"",ROUNDUP(K10+K10*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>3600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="111"/>
+      <c r="B11" s="97"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -2491,29 +2491,29 @@
       <c r="M11" s="6"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="111"/>
+      <c r="B12" s="97"/>
       <c r="C12" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="105" t="s">
+      <c r="D12" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="106"/>
-      <c r="F12" s="105" t="s">
+      <c r="E12" s="104"/>
+      <c r="F12" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="107"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="107"/>
-      <c r="J12" s="105" t="s">
+      <c r="G12" s="105"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="107"/>
-      <c r="L12" s="107"/>
-      <c r="M12" s="106"/>
+      <c r="K12" s="105"/>
+      <c r="L12" s="105"/>
+      <c r="M12" s="104"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="111"/>
+      <c r="B13" s="97"/>
       <c r="C13" s="10"/>
       <c r="D13" s="56" t="s">
         <v>13</v>
@@ -2521,25 +2521,25 @@
       <c r="E13" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="108" t="s">
+      <c r="F13" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="109"/>
-      <c r="H13" s="103" t="s">
+      <c r="G13" s="107"/>
+      <c r="H13" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="109"/>
-      <c r="J13" s="108" t="s">
+      <c r="I13" s="107"/>
+      <c r="J13" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="109"/>
-      <c r="L13" s="103" t="s">
+      <c r="K13" s="107"/>
+      <c r="L13" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="104"/>
+      <c r="M13" s="109"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="111"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="10"/>
       <c r="D14" s="56" t="s">
         <v>8</v>
@@ -2573,17 +2573,17 @@
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="111"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="46" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="48">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_CORE_AT,LO_CORE_AT)),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="50">
         <f>D15+D15*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="F15" s="48">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_CORE_AT,MEDIUM_CORE_AT)),0)</f>
@@ -2603,33 +2603,33 @@
       </c>
       <c r="J15" s="48">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_CORE_AT,0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15" s="51">
         <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_CORE_DT,MEDIUM_CORE_DT)),0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L15" s="52">
         <f>J15+J15*VIRTUAL_PERCENTAGE</f>
-        <v>2.4</v>
+        <v>0</v>
       </c>
       <c r="M15" s="53">
         <f>IF(K15&lt;&gt;"",ROUNDUP(K15+K15*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="111"/>
+      <c r="B16" s="97"/>
       <c r="C16" s="46" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="48">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_RAM_AT,LO_RAM_AT)),0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E16" s="50">
         <f>D16+D16*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="F16" s="48">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_RAM_AT,MEDIUM_RAM_AT)),0)</f>
@@ -2649,33 +2649,33 @@
       </c>
       <c r="J16" s="48">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_RAM_AT,0)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K16" s="51">
         <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_RAM_DT,MEDIUM_RAM_DT)),0)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L16" s="52">
         <f>J16+J16*VIRTUAL_PERCENTAGE</f>
-        <v>4.8</v>
+        <v>0</v>
       </c>
       <c r="M16" s="53">
         <f>IF(K16&lt;&gt;"",ROUNDUP(K16+K16*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="112"/>
+      <c r="B17" s="98"/>
       <c r="C17" s="47" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="49">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_DISK_AT,LO_DISK_AT)),0)</f>
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="E17" s="62">
         <f>D17+D17*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="F17" s="49">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,MEDIUM_DISK_AT,HI_DISK_AT)),0)</f>
@@ -2695,48 +2695,48 @@
       </c>
       <c r="J17" s="49">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_DISK_AT,0)</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="K17" s="54">
         <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_DISK_DT,MEDIUM_DISK_DT)),0)</f>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="L17" s="63">
         <f>J17+J17*VIRTUAL_PERCENTAGE</f>
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="M17" s="55">
         <f>IF(K17&lt;&gt;"",ROUNDUP(K17+K17*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>2400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="113" t="s">
-        <v>56</v>
+      <c r="B20" s="99" t="s">
+        <v>55</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="105" t="s">
+      <c r="D20" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="106"/>
-      <c r="F20" s="105" t="s">
+      <c r="E20" s="104"/>
+      <c r="F20" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="107"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="106"/>
-      <c r="J20" s="105" t="s">
+      <c r="G20" s="105"/>
+      <c r="H20" s="105"/>
+      <c r="I20" s="104"/>
+      <c r="J20" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="107"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="106"/>
+      <c r="K20" s="105"/>
+      <c r="L20" s="105"/>
+      <c r="M20" s="104"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="114"/>
+      <c r="B21" s="100"/>
       <c r="C21" s="3"/>
       <c r="D21" s="56" t="s">
         <v>13</v>
@@ -2744,25 +2744,25 @@
       <c r="E21" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="108" t="s">
+      <c r="F21" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="109"/>
-      <c r="H21" s="103" t="s">
+      <c r="G21" s="107"/>
+      <c r="H21" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="104"/>
-      <c r="J21" s="108" t="s">
+      <c r="I21" s="109"/>
+      <c r="J21" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="109"/>
-      <c r="L21" s="103" t="s">
+      <c r="K21" s="107"/>
+      <c r="L21" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="M21" s="104"/>
+      <c r="M21" s="109"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="114"/>
+      <c r="B22" s="100"/>
       <c r="C22" s="3"/>
       <c r="D22" s="56" t="s">
         <v>8</v>
@@ -2796,7 +2796,7 @@
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="114"/>
+      <c r="B23" s="100"/>
       <c r="C23" s="4" t="s">
         <v>17</v>
       </c>
@@ -2826,23 +2826,23 @@
       </c>
       <c r="J23" s="48">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K23" s="17">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L23" s="52">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M23" s="53">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="114"/>
+      <c r="B24" s="100"/>
       <c r="C24" s="4" t="s">
         <v>18</v>
       </c>
@@ -2872,23 +2872,23 @@
       </c>
       <c r="J24" s="48">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K24" s="17">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="L24" s="52">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M24" s="53">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="114"/>
+      <c r="B25" s="100"/>
       <c r="C25" s="5" t="s">
         <v>19</v>
       </c>
@@ -2918,23 +2918,23 @@
       </c>
       <c r="J25" s="49">
         <f t="shared" si="2"/>
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="K25" s="18">
         <f t="shared" si="2"/>
-        <v>3750</v>
+        <v>0</v>
       </c>
       <c r="L25" s="63">
         <f t="shared" si="2"/>
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="M25" s="55">
         <f t="shared" si="2"/>
-        <v>4500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="114"/>
+      <c r="B26" s="100"/>
       <c r="D26" s="61"/>
       <c r="E26" s="61"/>
       <c r="F26" s="61"/>
@@ -2947,29 +2947,29 @@
       <c r="M26" s="61"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="114"/>
+      <c r="B27" s="100"/>
       <c r="C27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="105" t="s">
+      <c r="D27" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="106"/>
-      <c r="F27" s="105" t="s">
+      <c r="E27" s="104"/>
+      <c r="F27" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="107"/>
-      <c r="H27" s="107"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="105" t="s">
+      <c r="G27" s="105"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="104"/>
+      <c r="J27" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="K27" s="107"/>
-      <c r="L27" s="107"/>
-      <c r="M27" s="106"/>
+      <c r="K27" s="105"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="104"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="114"/>
+      <c r="B28" s="100"/>
       <c r="C28" s="3"/>
       <c r="D28" s="56" t="s">
         <v>13</v>
@@ -2977,25 +2977,25 @@
       <c r="E28" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="F28" s="108" t="s">
+      <c r="F28" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="G28" s="109"/>
-      <c r="H28" s="103" t="s">
+      <c r="G28" s="107"/>
+      <c r="H28" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="I28" s="104"/>
-      <c r="J28" s="108" t="s">
+      <c r="I28" s="109"/>
+      <c r="J28" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="K28" s="109"/>
-      <c r="L28" s="103" t="s">
+      <c r="K28" s="107"/>
+      <c r="L28" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="M28" s="104"/>
+      <c r="M28" s="109"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="114"/>
+      <c r="B29" s="100"/>
       <c r="C29" s="3"/>
       <c r="D29" s="56" t="s">
         <v>8</v>
@@ -3029,17 +3029,17 @@
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="114"/>
+      <c r="B30" s="100"/>
       <c r="C30" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="48">
         <f t="shared" ref="D30:M30" si="3">ROUNDUP(D15+D15*BEEF_FACTOR,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E30" s="50">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30" s="48">
         <f t="shared" si="3"/>
@@ -3059,33 +3059,33 @@
       </c>
       <c r="J30" s="48">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K30" s="17">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L30" s="52">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M30" s="53">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="114"/>
+      <c r="B31" s="100"/>
       <c r="C31" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="48">
         <f t="shared" ref="D31:M31" si="4">ROUNDUP(D16+D16*BEEF_FACTOR,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E31" s="50">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F31" s="48">
         <f t="shared" si="4"/>
@@ -3105,33 +3105,33 @@
       </c>
       <c r="J31" s="48">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K31" s="17">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L31" s="52">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M31" s="53">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="115"/>
+      <c r="B32" s="101"/>
       <c r="C32" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="49">
         <f t="shared" ref="D32:M32" si="5">ROUNDUP(D17+D17*BEEF_FACTOR,0)</f>
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="E32" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>188</v>
       </c>
       <c r="F32" s="49">
         <f t="shared" si="5"/>
@@ -3151,24 +3151,39 @@
       </c>
       <c r="J32" s="49">
         <f t="shared" si="5"/>
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="K32" s="18">
         <f t="shared" si="5"/>
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="L32" s="63">
         <f t="shared" si="5"/>
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="M32" s="55">
         <f t="shared" si="5"/>
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="31">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
     <mergeCell ref="B5:B17"/>
     <mergeCell ref="B20:B32"/>
     <mergeCell ref="B2:M2"/>
@@ -3185,21 +3200,6 @@
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="H21:I21"/>
     <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
   </mergeCells>
   <conditionalFormatting sqref="D5:M32">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
@@ -3528,15 +3528,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <Project xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">45</Project>
@@ -3545,6 +3536,15 @@
     <Review_x0020_Status xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">Review Completed</Review_x0020_Status>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3565,18 +3565,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C0D350-2871-401C-8D5C-791C478D9E13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312B28CD-EB51-4560-8E58-B9E03DAFD80D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="d4f1fd26-cd3f-48df-8559-6269d85163e3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C0D350-2871-401C-8D5C-791C478D9E13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add reviewers and "dated" warning in workbook. (#67)
* Add reviewers and "dated" warning in workbook.
* Fix "architecture" typo.
* Update capacity workbook

Merging the PR, so that we can start work on the final article.
</commit_message>
<xml_diff>
--- a/src/Planning/understand-options-tfs-vsts-environments-capacity-guide.xlsx
+++ b/src/Planning/understand-options-tfs-vsts-environments-capacity-guide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willy\OneDrive\_sandbox\planning guide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willy\OneDrive\_repos\Guidance\src\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_481838BC9F82B1C870C8F03207606A56245E0862" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{B660518E-83CE-48D7-B6B4-7AF39787574A}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{2807C006-C69B-4AC9-8D01-14B79F4CDF28}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{B2CD11E7-C4ED-4C84-8FBA-E50379023EA9}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="7812" windowWidth="21840" windowHeight="7272" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12" yWindow="9180" windowWidth="21840" windowHeight="7272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server Scenarios" sheetId="1" r:id="rId1"/>
@@ -48,6 +48,8 @@
     <definedName name="MEDIUM_DISK_DT">Constants!$K$4</definedName>
     <definedName name="MEDIUM_RAM_AT">Constants!$G$4</definedName>
     <definedName name="MEDIUM_RAM_DT">Constants!$J$4</definedName>
+    <definedName name="MEDIUM_RPS">Constants!$B$4</definedName>
+    <definedName name="MEDIUM_TPC">Constants!$E$4</definedName>
     <definedName name="MEDIUM_USERS">Constants!$C$4</definedName>
     <definedName name="SCALE_CORE_AT">Constants!$F$6</definedName>
     <definedName name="SCALE_CORE_DT">Constants!$I$6</definedName>
@@ -73,12 +75,12 @@
     <definedName name="STANDARD_USERS">Constants!$C$3</definedName>
     <definedName name="VIRTUAL_PERCENTAGE">Constants!$B$19</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="60">
   <si>
     <t>F</t>
   </si>
@@ -147,42 +149,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NOTE:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This is a simplified model for educational purposes and does not replace expert consulting. Real world requirements and infrastructure environments can be much more complex.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -331,9 +297,6 @@
     <t>Virtual Percentage</t>
   </si>
   <si>
-    <t>Medium-End Configurtion</t>
-  </si>
-  <si>
     <t>RAM-DT</t>
   </si>
   <si>
@@ -350,9 +313,6 @@
   </si>
   <si>
     <t>DISK-DT</t>
-  </si>
-  <si>
-    <t>Review the Real-World “Beef” Factor section in the TFS Project Guidance document.</t>
   </si>
   <si>
     <t>BETA</t>
@@ -411,9 +371,6 @@
       </rPr>
       <t xml:space="preserve"> FACTOR</t>
     </r>
-  </si>
-  <si>
-    <t>Version 2012.02.24</t>
   </si>
   <si>
     <r>
@@ -451,12 +408,70 @@
       <t>This is a simplified model for educational purposes and does not replace expert consulting. Real-world requirements and infrastructure environments can be much more complex.</t>
     </r>
   </si>
+  <si>
+    <t>Safety growth factor to add to proposed architecture.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTE: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This is a simplified model for educational purposes and does not replace expert consulting. Real world requirements and infrastructure environments can be much more complex.</t>
+    </r>
+  </si>
+  <si>
+    <t>Version 2018.08.03</t>
+  </si>
+  <si>
+    <t>Medium-End Configuration</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Read </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://docs.microsoft.com/en-us/tfs/server/requirements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for up-to-date operating system, hardware, virtualization, and other requirements.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,6 +633,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -976,7 +998,7 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1145,6 +1167,69 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1163,108 +1248,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1286,6 +1269,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1367,7 +1393,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>2990938</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>908550</xdr:rowOff>
+      <xdr:rowOff>899025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1732,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1754,60 +1780,60 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="75"/>
+      <c r="A5" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="95" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="96"/>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="1.65">
-      <c r="A6" s="70"/>
+      <c r="A6" s="91"/>
       <c r="B6" s="66" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="67">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>1</v>
       </c>
       <c r="I6" s="64" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="71"/>
+      <c r="A7" s="92"/>
       <c r="B7" s="68" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="69">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>3</v>
@@ -1822,13 +1848,13 @@
     <row r="9" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22"/>
       <c r="B9" s="25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="16">
         <v>0.25</v>
       </c>
-      <c r="D9" s="26" t="s">
-        <v>52</v>
+      <c r="E9" s="26" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1838,115 +1864,115 @@
       <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76" t="s">
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76" t="s">
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="76"/>
-      <c r="K11" s="94"/>
+      <c r="J11" s="83"/>
+      <c r="K11" s="84"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="73"/>
-      <c r="C12" s="77" t="s">
+      <c r="B12" s="94"/>
+      <c r="C12" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77" t="s">
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77" t="s">
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="77"/>
-      <c r="K12" s="95"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="86"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="80" t="str">
+      <c r="C13" s="87" t="str">
         <f>IF(Current_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80" t="str">
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87" t="str">
         <f>IF(Current_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80" t="str">
+      <c r="G13" s="87"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87" t="str">
         <f>I14</f>
-        <v>Yes</v>
-      </c>
-      <c r="J13" s="80"/>
-      <c r="K13" s="83"/>
+        <v>No</v>
+      </c>
+      <c r="J13" s="87"/>
+      <c r="K13" s="88"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="81" t="str">
+      <c r="C14" s="89" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
-        <v>No</v>
-      </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="D14" s="89"/>
+      <c r="E14" s="89"/>
+      <c r="F14" s="89" t="str">
         <f>IF(Future_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81" t="str">
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
+      <c r="I14" s="89" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_YES,C_NO)</f>
-        <v>Yes</v>
-      </c>
-      <c r="J14" s="81"/>
-      <c r="K14" s="84"/>
+        <v>No</v>
+      </c>
+      <c r="J14" s="89"/>
+      <c r="K14" s="90"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="81" t="str">
+      <c r="C15" s="89" t="str">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;1),C_YES,C_NO)</f>
-        <v>No</v>
-      </c>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81" t="str">
+        <v>Yes</v>
+      </c>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;1),C_YES,C_NO)</f>
         <v>Yes</v>
       </c>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="81" t="str">
+      <c r="G15" s="89"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="89" t="str">
         <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),C_YES,C_NO)</f>
-        <v>Yes</v>
-      </c>
-      <c r="J15" s="81"/>
-      <c r="K15" s="84"/>
+        <v>No</v>
+      </c>
+      <c r="J15" s="89"/>
+      <c r="K15" s="90"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="29" t="str">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
@@ -1954,162 +1980,162 @@
       </c>
       <c r="D16" s="30" t="str">
         <f>IF(E16="","","-")</f>
-        <v/>
+        <v>-</v>
       </c>
       <c r="E16" s="31" t="str">
         <f>IF(C14=C_YES,(IF(Future_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
-        <v/>
-      </c>
-      <c r="F16" s="82" t="str">
+        <v>Low-End</v>
+      </c>
+      <c r="F16" s="72" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),"High-End","")</f>
         <v>High-End</v>
       </c>
-      <c r="G16" s="82"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="82" t="str">
-        <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),"Scale Unit","")</f>
-        <v>Scale Unit</v>
-      </c>
-      <c r="J16" s="82"/>
-      <c r="K16" s="86"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="72" t="str">
+        <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),"Scale Unit","")</f>
+        <v/>
+      </c>
+      <c r="J16" s="72"/>
+      <c r="K16" s="73"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="78">
+        <v>39</v>
+      </c>
+      <c r="C17" s="74">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
         <v>5</v>
       </c>
-      <c r="D17" s="78"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78">
+      <c r="D17" s="74"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="74">
         <f>IF(F13=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78">
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74" t="str">
         <f>IF(I13=C_YES,SCALE_TPC,"")</f>
-        <v>75</v>
-      </c>
-      <c r="J17" s="78"/>
-      <c r="K17" s="91"/>
+        <v/>
+      </c>
+      <c r="J17" s="74"/>
+      <c r="K17" s="79"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="79">
+        <v>40</v>
+      </c>
+      <c r="C18" s="80">
         <f>IF(C13=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
-        <v>10</v>
-      </c>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="78">
+        <v>5</v>
+      </c>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="74">
         <f>IF(F14=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G18" s="78"/>
-      <c r="H18" s="78"/>
-      <c r="I18" s="79">
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="80" t="str">
         <f>IF(I14=C_YES,SCALE_TPC,"")</f>
-        <v>75</v>
-      </c>
-      <c r="J18" s="79"/>
-      <c r="K18" s="92"/>
+        <v/>
+      </c>
+      <c r="J18" s="80"/>
+      <c r="K18" s="81"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="93">
+        <v>37</v>
+      </c>
+      <c r="C19" s="82">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93">
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="G19" s="93"/>
-      <c r="H19" s="93"/>
-      <c r="I19" s="34">
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="34" t="str">
         <f>IF(I13=C_YES,ROUNDUP(I20/SCALE_RPS,0),"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="J19" s="35" t="str">
         <f>IF(K19&lt;&gt;"","-","")</f>
-        <v>-</v>
-      </c>
-      <c r="K19" s="36">
+        <v/>
+      </c>
+      <c r="K19" s="36" t="str">
         <f>IF(I14=C_YES,ROUNDUP(K20/SCALE_RPS,0),"")</f>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="87">
+        <v>42</v>
+      </c>
+      <c r="C20" s="75">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,Current_Users*STANDARD_FACTOR,Current_Users*LO_FACTOR)),"")</f>
-        <v>35</v>
-      </c>
-      <c r="D20" s="87" t="str">
+        <v>0</v>
+      </c>
+      <c r="D20" s="75" t="str">
         <f>IF(E20&lt;&gt;"","-","")</f>
-        <v/>
-      </c>
-      <c r="E20" s="87" t="str">
+        <v>-</v>
+      </c>
+      <c r="E20" s="75">
         <f>IF(C14=C_YES,(IF(Future_Users&gt;LO_USERS,Future_Users*STANDARD_FACTOR,Future_Users*LO_FACTOR)),"")</f>
-        <v/>
-      </c>
-      <c r="F20" s="89">
+        <v>0</v>
+      </c>
+      <c r="F20" s="77">
         <f>IF(F13=C_YES,Current_Users*HI_FACTOR,"")</f>
-        <v>45</v>
-      </c>
-      <c r="G20" s="87" t="str">
+        <v>0</v>
+      </c>
+      <c r="G20" s="75" t="str">
         <f>IF(H20&lt;&gt;"","-","")</f>
         <v>-</v>
       </c>
-      <c r="H20" s="89">
+      <c r="H20" s="77">
         <f>IF(F14=C_YES,Future_Users*HI_FACTOR,"")</f>
-        <v>450</v>
-      </c>
-      <c r="I20" s="37">
+        <v>0</v>
+      </c>
+      <c r="I20" s="37" t="str">
         <f>IF(I13=C_YES,Current_Users*SCALE_FACTOR,"")</f>
-        <v>52.5</v>
+        <v/>
       </c>
       <c r="J20" s="38" t="str">
         <f>IF(K20&lt;&gt;"","-","")</f>
-        <v>-</v>
-      </c>
-      <c r="K20" s="39">
+        <v/>
+      </c>
+      <c r="K20" s="39" t="str">
         <f>IF(I13=C_YES,Future_Users*HI_FACTOR,"")</f>
-        <v>450</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
-      <c r="E21" s="88"/>
-      <c r="F21" s="90"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="90"/>
-      <c r="I21" s="41">
+        <v>36</v>
+      </c>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="41" t="str">
         <f>IF(I13=C_YES,I20/I19,"")</f>
-        <v>52.5</v>
+        <v/>
       </c>
       <c r="J21" s="42" t="str">
         <f>IF(K21&lt;&gt;"","-","")</f>
-        <v>-</v>
-      </c>
-      <c r="K21" s="43">
+        <v/>
+      </c>
+      <c r="K21" s="43" t="str">
         <f>IF(I14=C_YES,K20/K19,"")</f>
-        <v>450</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="2:11" ht="91.8" x14ac:dyDescent="1.65">
@@ -2117,6 +2143,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="F17:H17"/>
@@ -2133,25 +2178,6 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="I12:K12"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
     <cfRule type="expression" dxfId="7" priority="13">
@@ -2171,7 +2197,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
+  <conditionalFormatting sqref="E9">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$C$9&gt;0</formula>
     </cfRule>
@@ -2213,10 +2239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:M32"/>
+  <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2229,984 +2255,990 @@
   <sheetData>
     <row r="1" spans="2:13" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="116" t="str">
+      <c r="B2" s="103" t="str">
         <f>'Server Scenarios'!B2:K2</f>
-        <v>Version 2012.02.24</v>
-      </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
+        <v>Version 2018.08.03</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" s="118" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="110" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="96" t="s">
+      <c r="D6" s="111" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="97"/>
-      <c r="F5" s="96" t="s">
+      <c r="E6" s="112"/>
+      <c r="F6" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="96" t="s">
+      <c r="G6" s="113"/>
+      <c r="H6" s="113"/>
+      <c r="I6" s="113"/>
+      <c r="J6" s="111" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="97"/>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="111"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="99" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="100"/>
-      <c r="H6" s="101" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="100"/>
-      <c r="J6" s="99" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="100"/>
-      <c r="L6" s="101" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="102"/>
+      <c r="K6" s="113"/>
+      <c r="L6" s="113"/>
+      <c r="M6" s="112"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="111"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="3"/>
       <c r="D7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="114" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="115"/>
+      <c r="H7" s="116" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="115"/>
+      <c r="J7" s="114" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="115"/>
+      <c r="L7" s="116" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="117"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B8" s="98"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="L8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="M8" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="111"/>
-      <c r="C8" s="4" t="s">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B9" s="98"/>
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D9" s="48">
         <f>IF(SINGLE_CURRENT_OK=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_CORE_AT,LO_CORE_AT)),0)</f>
         <v>1</v>
       </c>
-      <c r="E8" s="50">
-        <f>IFD8+D8*VIRTUAL_PERCENTAGE</f>
+      <c r="E9" s="50">
+        <f>IFD9+D9*VIRTUAL_PERCENTAGE</f>
         <v>0.2</v>
       </c>
-      <c r="F8" s="48">
+      <c r="F9" s="48">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_CORE_AT,MEDIUM_CORE_AT)),0)</f>
         <v>2</v>
       </c>
-      <c r="G8" s="51">
+      <c r="G9" s="51">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_CORE_DT,MEDIUM_CORE_DT)),0)</f>
         <v>4</v>
       </c>
-      <c r="H8" s="52">
-        <f>F8+F8*VIRTUAL_PERCENTAGE</f>
+      <c r="H9" s="52">
+        <f>F9+F9*VIRTUAL_PERCENTAGE</f>
         <v>2.4</v>
       </c>
-      <c r="I8" s="17">
-        <f>IF(G8&lt;&gt;"",ROUNDUP(G8+G8*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="I9" s="17">
+        <f>IF(G9&lt;&gt;"",ROUNDUP(G9+G9*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>5</v>
       </c>
-      <c r="J8" s="48">
+      <c r="J9" s="48">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_CORE_AT,0)</f>
-        <v>2</v>
-      </c>
-      <c r="K8" s="51">
-        <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_CORE_DT,HI_CORE_DT)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="51">
+        <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;SCALE_USERS,SCALE_CORE_DT,SCALE_CORE_DT)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="52">
+        <f>J9+J9*VIRTUAL_PERCENTAGE</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="53">
+        <f>IF(K9&lt;&gt;"",ROUNDUP(K9+K9*VIRTUAL_PERCENTAGE,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B10" s="98"/>
+      <c r="C10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="48">
+        <f>IF(SINGLE_CURRENT_OK=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_RAM_AT,LO_RAM_AT)),0)</f>
+        <v>4</v>
+      </c>
+      <c r="E10" s="50">
+        <f>D10+D10*VIRTUAL_PERCENTAGE</f>
+        <v>4.8</v>
+      </c>
+      <c r="F10" s="48">
+        <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_RAM_AT,MEDIUM_RAM_AT)),0)</f>
         <v>8</v>
       </c>
-      <c r="L8" s="52">
-        <f>J8+J8*VIRTUAL_PERCENTAGE</f>
-        <v>2.4</v>
-      </c>
-      <c r="M8" s="53">
-        <f>IF(K8&lt;&gt;"",ROUNDUP(K8+K8*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="111"/>
-      <c r="C9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="48">
-        <f>IF(SINGLE_CURRENT_OK=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_RAM_AT,LO_RAM_AT)),0)</f>
-        <v>2</v>
-      </c>
-      <c r="E9" s="50">
-        <f>D9+D9*VIRTUAL_PERCENTAGE</f>
-        <v>2.4</v>
-      </c>
-      <c r="F9" s="48">
-        <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_RAM_AT,MEDIUM_RAM_AT)),0)</f>
-        <v>4</v>
-      </c>
-      <c r="G9" s="51">
+      <c r="G10" s="51">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_RAM_DT,MEDIUM_RAM_DT)),0)</f>
         <v>8</v>
       </c>
-      <c r="H9" s="52">
-        <f>F9+F9*VIRTUAL_PERCENTAGE</f>
-        <v>4.8</v>
-      </c>
-      <c r="I9" s="17">
-        <f>IF(G9&lt;&gt;"",ROUNDUP(G9+G9*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="H10" s="52">
+        <f>F10+F10*VIRTUAL_PERCENTAGE</f>
+        <v>9.6</v>
+      </c>
+      <c r="I10" s="17">
+        <f>IF(G10&lt;&gt;"",ROUNDUP(G10+G10*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>10</v>
       </c>
-      <c r="J9" s="48">
+      <c r="J10" s="48">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_RAM_AT,0)</f>
-        <v>4</v>
-      </c>
-      <c r="K9" s="51">
-        <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_RAM_DT,HI_RAM_DT)),0)</f>
-        <v>16</v>
-      </c>
-      <c r="L9" s="52">
-        <f>J9+J9*VIRTUAL_PERCENTAGE</f>
-        <v>4.8</v>
-      </c>
-      <c r="M9" s="53">
-        <f>IF(K9&lt;&gt;"",ROUNDUP(K9+K9*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="111"/>
-      <c r="C10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="51">
+        <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;SCALE_USERS,SCALE_RAM_DT,SCALE_RAM_DT)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="52">
+        <f>J10+J10*VIRTUAL_PERCENTAGE</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="53">
+        <f>IF(K10&lt;&gt;"",ROUNDUP(K10+K10*VIRTUAL_PERCENTAGE,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="98"/>
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="49">
+      <c r="D11" s="49">
         <f>IF(SINGLE_CURRENT_OK=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_DISK_AT,LO_DISK_AT)),0)</f>
         <v>125</v>
       </c>
-      <c r="E10" s="62">
-        <f>D10+D10*VIRTUAL_PERCENTAGE</f>
+      <c r="E11" s="62">
+        <f>D11+D11*VIRTUAL_PERCENTAGE</f>
         <v>150</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F11" s="49">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_DISK_AT,MEDIUM_DISK_AT)),0)</f>
         <v>500</v>
       </c>
-      <c r="G10" s="54">
+      <c r="G11" s="54">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_DISK_DT,MEDIUM_DISK_DT)),0)</f>
         <v>2000</v>
       </c>
-      <c r="H10" s="63">
-        <f>F10+F10*VIRTUAL_PERCENTAGE</f>
+      <c r="H11" s="63">
+        <f>F11+F11*VIRTUAL_PERCENTAGE</f>
         <v>600</v>
       </c>
-      <c r="I10" s="18">
-        <f>IF(G10&lt;&gt;"",ROUNDUP(G10+G10*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="I11" s="18">
+        <f>IF(G11&lt;&gt;"",ROUNDUP(G11+G11*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>2400</v>
       </c>
-      <c r="J10" s="49">
+      <c r="J11" s="49">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_DISK_AT,0)</f>
-        <v>500</v>
-      </c>
-      <c r="K10" s="54">
-        <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_DISK_DT,HI_DISK_DT)),0)</f>
-        <v>3000</v>
-      </c>
-      <c r="L10" s="63">
-        <f>J10+J10*VIRTUAL_PERCENTAGE</f>
-        <v>600</v>
-      </c>
-      <c r="M10" s="55">
-        <f>IF(K10&lt;&gt;"",ROUNDUP(K10+K10*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="111"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="111"/>
-      <c r="C12" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="K11" s="54">
+        <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;SCALE_USERS,SCALE_DISK_DT,SCALE_DISK_DT)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="63">
+        <f>J11+J11*VIRTUAL_PERCENTAGE</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="55">
+        <f>IF(K11&lt;&gt;"",ROUNDUP(K11+K11*VIRTUAL_PERCENTAGE,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="98"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B13" s="98"/>
+      <c r="C13" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="106"/>
-      <c r="F12" s="105" t="s">
+      <c r="E13" s="105"/>
+      <c r="F13" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="107"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="107"/>
-      <c r="J12" s="105" t="s">
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="107"/>
-      <c r="L12" s="107"/>
-      <c r="M12" s="106"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="111"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="108" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="109"/>
-      <c r="H13" s="103" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="109"/>
-      <c r="J13" s="108" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="109"/>
-      <c r="L13" s="103" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="104"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="106"/>
+      <c r="M13" s="105"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="111"/>
+      <c r="B14" s="98"/>
       <c r="C14" s="10"/>
       <c r="D14" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="107" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="108"/>
+      <c r="H14" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="108"/>
+      <c r="J14" s="107" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="108"/>
+      <c r="L14" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="110"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="98"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E15" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="56" t="s">
+      <c r="F15" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="58" t="s">
+      <c r="G15" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="59" t="s">
+      <c r="H15" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="58" t="s">
+      <c r="I15" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="56" t="s">
+      <c r="J15" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="58" t="s">
+      <c r="K15" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="L14" s="59" t="s">
+      <c r="L15" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="60" t="s">
+      <c r="M15" s="60" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="111"/>
-      <c r="C15" s="46" t="s">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B16" s="98"/>
+      <c r="C16" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D16" s="48">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_CORE_AT,LO_CORE_AT)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="50">
-        <f>D15+D15*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="48">
+        <v>1</v>
+      </c>
+      <c r="E16" s="50">
+        <f>D16+D16*VIRTUAL_PERCENTAGE</f>
+        <v>1.2</v>
+      </c>
+      <c r="F16" s="48">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_CORE_AT,MEDIUM_CORE_AT)),0)</f>
         <v>2</v>
       </c>
-      <c r="G15" s="51">
+      <c r="G16" s="51">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_CORE_DT,MEDIUM_CORE_DT)),0)</f>
         <v>4</v>
       </c>
-      <c r="H15" s="52">
-        <f>F15+F15*VIRTUAL_PERCENTAGE</f>
+      <c r="H16" s="52">
+        <f>F16+F16*VIRTUAL_PERCENTAGE</f>
         <v>2.4</v>
       </c>
-      <c r="I15" s="17">
-        <f>IF(G15&lt;&gt;"",ROUNDUP(G15+G15*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="I16" s="17">
+        <f>IF(G16&lt;&gt;"",ROUNDUP(G16+G16*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>5</v>
       </c>
-      <c r="J15" s="48">
+      <c r="J16" s="48">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_CORE_AT,0)</f>
-        <v>2</v>
-      </c>
-      <c r="K15" s="51">
-        <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_CORE_DT,MEDIUM_CORE_DT)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="51">
+        <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;SCALE_USERS,SCALE_CORE_DT,SCALE_CORE_DT)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="52">
+        <f>J16+J16*VIRTUAL_PERCENTAGE</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="53">
+        <f>IF(K16&lt;&gt;"",ROUNDUP(K16+K16*VIRTUAL_PERCENTAGE,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B17" s="98"/>
+      <c r="C17" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="48">
+        <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_RAM_AT,LO_RAM_AT)),0)</f>
         <v>4</v>
       </c>
-      <c r="L15" s="52">
-        <f>J15+J15*VIRTUAL_PERCENTAGE</f>
-        <v>2.4</v>
-      </c>
-      <c r="M15" s="53">
-        <f>IF(K15&lt;&gt;"",ROUNDUP(K15+K15*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="111"/>
-      <c r="C16" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="48">
-        <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_RAM_AT,LO_RAM_AT)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="50">
-        <f>D16+D16*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="48">
+      <c r="E17" s="50">
+        <f>D17+D17*VIRTUAL_PERCENTAGE</f>
+        <v>4.8</v>
+      </c>
+      <c r="F17" s="48">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_RAM_AT,MEDIUM_RAM_AT)),0)</f>
-        <v>4</v>
-      </c>
-      <c r="G16" s="51">
+        <v>8</v>
+      </c>
+      <c r="G17" s="51">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_RAM_DT,MEDIUM_RAM_DT)),0)</f>
         <v>8</v>
       </c>
-      <c r="H16" s="52">
-        <f>F16+F16*VIRTUAL_PERCENTAGE</f>
-        <v>4.8</v>
-      </c>
-      <c r="I16" s="17">
-        <f>IF(G16&lt;&gt;"",ROUNDUP(G16+G16*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="H17" s="52">
+        <f>F17+F17*VIRTUAL_PERCENTAGE</f>
+        <v>9.6</v>
+      </c>
+      <c r="I17" s="17">
+        <f>IF(G17&lt;&gt;"",ROUNDUP(G17+G17*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>10</v>
       </c>
-      <c r="J16" s="48">
+      <c r="J17" s="48">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_RAM_AT,0)</f>
-        <v>4</v>
-      </c>
-      <c r="K16" s="51">
-        <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_RAM_DT,MEDIUM_RAM_DT)),0)</f>
-        <v>8</v>
-      </c>
-      <c r="L16" s="52">
-        <f>J16+J16*VIRTUAL_PERCENTAGE</f>
-        <v>4.8</v>
-      </c>
-      <c r="M16" s="53">
-        <f>IF(K16&lt;&gt;"",ROUNDUP(K16+K16*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="112"/>
-      <c r="C17" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="51">
+        <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;SCALE_USERS,SCALE_RAM_DT,SCALE_RAM_DT)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="52">
+        <f>J17+J17*VIRTUAL_PERCENTAGE</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="53">
+        <f>IF(K17&lt;&gt;"",ROUNDUP(K17+K17*VIRTUAL_PERCENTAGE,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="99"/>
+      <c r="C18" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D18" s="49">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_DISK_AT,LO_DISK_AT)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="62">
-        <f>D17+D17*VIRTUAL_PERCENTAGE</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="49">
+        <v>125</v>
+      </c>
+      <c r="E18" s="62">
+        <f>D18+D18*VIRTUAL_PERCENTAGE</f>
+        <v>150</v>
+      </c>
+      <c r="F18" s="49">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,MEDIUM_DISK_AT,HI_DISK_AT)),0)</f>
         <v>500</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G18" s="54">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_DISK_DT,MEDIUM_DISK_DT)),0)</f>
         <v>2000</v>
       </c>
-      <c r="H17" s="63">
-        <f>F17+F17*VIRTUAL_PERCENTAGE</f>
+      <c r="H18" s="63">
+        <f>F18+F18*VIRTUAL_PERCENTAGE</f>
         <v>600</v>
       </c>
-      <c r="I17" s="18">
-        <f>IF(G17&lt;&gt;"",ROUNDUP(G17+G17*VIRTUAL_PERCENTAGE,0),0)</f>
+      <c r="I18" s="18">
+        <f>IF(G18&lt;&gt;"",ROUNDUP(G18+G18*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>2400</v>
       </c>
-      <c r="J17" s="49">
+      <c r="J18" s="49">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_DISK_AT,0)</f>
-        <v>500</v>
-      </c>
-      <c r="K17" s="54">
-        <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_DISK_DT,MEDIUM_DISK_DT)),0)</f>
-        <v>2000</v>
-      </c>
-      <c r="L17" s="63">
-        <f>J17+J17*VIRTUAL_PERCENTAGE</f>
-        <v>600</v>
-      </c>
-      <c r="M17" s="55">
-        <f>IF(K17&lt;&gt;"",ROUNDUP(K17+K17*VIRTUAL_PERCENTAGE,0),0)</f>
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="113" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="105" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="54">
+        <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;SCALE_USERS,SCALE_DISK_DT,SCALE_DISK_DT)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L18" s="63">
+        <f>J18+J18*VIRTUAL_PERCENTAGE</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="55">
+        <f>IF(K18&lt;&gt;"",ROUNDUP(K18+K18*VIRTUAL_PERCENTAGE,0),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B21" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="106"/>
-      <c r="F20" s="105" t="s">
+      <c r="E21" s="105"/>
+      <c r="F21" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="107"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="106"/>
-      <c r="J20" s="105" t="s">
+      <c r="G21" s="106"/>
+      <c r="H21" s="106"/>
+      <c r="I21" s="105"/>
+      <c r="J21" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="107"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="106"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="114"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="108" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="109"/>
-      <c r="H21" s="103" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="104"/>
-      <c r="J21" s="108" t="s">
-        <v>13</v>
-      </c>
-      <c r="K21" s="109"/>
-      <c r="L21" s="103" t="s">
-        <v>14</v>
-      </c>
-      <c r="M21" s="104"/>
+      <c r="K21" s="106"/>
+      <c r="L21" s="106"/>
+      <c r="M21" s="105"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="114"/>
+      <c r="B22" s="101"/>
       <c r="C22" s="3"/>
       <c r="D22" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="107" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="108"/>
+      <c r="H22" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="110"/>
+      <c r="J22" s="107" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="108"/>
+      <c r="L22" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" s="110"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="101"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="57" t="s">
+      <c r="E23" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="56" t="s">
+      <c r="F23" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="58" t="s">
+      <c r="G23" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="59" t="s">
+      <c r="H23" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="I22" s="60" t="s">
+      <c r="I23" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="J22" s="56" t="s">
+      <c r="J23" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="58" t="s">
+      <c r="K23" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="59" t="s">
+      <c r="L23" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="M22" s="60" t="s">
+      <c r="M23" s="60" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="114"/>
-      <c r="C23" s="4" t="s">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B24" s="101"/>
+      <c r="C24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="48">
-        <f t="shared" ref="D23:M23" si="0">ROUNDUP(D8+D8*BEEF_FACTOR,0)</f>
+      <c r="D24" s="48">
+        <f t="shared" ref="D24:M24" si="0">ROUNDUP(D9+D9*BEEF_FACTOR,0)</f>
         <v>2</v>
       </c>
-      <c r="E23" s="50">
+      <c r="E24" s="50">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F23" s="48">
+      <c r="F24" s="48">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G24" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H23" s="52">
+      <c r="H24" s="52">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I23" s="53">
+      <c r="I24" s="53">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J23" s="48">
+      <c r="J24" s="48">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="K23" s="17">
+        <v>0</v>
+      </c>
+      <c r="K24" s="17">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="L23" s="52">
+        <v>0</v>
+      </c>
+      <c r="L24" s="52">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="M23" s="53">
+        <v>0</v>
+      </c>
+      <c r="M24" s="53">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="114"/>
-      <c r="C24" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B25" s="101"/>
+      <c r="C25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="48">
-        <f t="shared" ref="D24:M24" si="1">ROUNDUP(D9+D9*BEEF_FACTOR,0)</f>
-        <v>3</v>
-      </c>
-      <c r="E24" s="50">
+      <c r="D25" s="48">
+        <f t="shared" ref="D25:M25" si="1">ROUNDUP(D10+D10*BEEF_FACTOR,0)</f>
+        <v>5</v>
+      </c>
+      <c r="E25" s="50">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F24" s="48">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G24" s="17">
+        <v>6</v>
+      </c>
+      <c r="F25" s="48">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H24" s="52">
+      <c r="G25" s="17">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="I24" s="53">
+        <v>10</v>
+      </c>
+      <c r="H25" s="52">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I25" s="53">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J24" s="48">
+      <c r="J25" s="48">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="K24" s="17">
+        <v>0</v>
+      </c>
+      <c r="K25" s="17">
         <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="L24" s="52">
+        <v>0</v>
+      </c>
+      <c r="L25" s="52">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="M24" s="53">
+        <v>0</v>
+      </c>
+      <c r="M25" s="53">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="114"/>
-      <c r="C25" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="101"/>
+      <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="49">
-        <f t="shared" ref="D25:M25" si="2">ROUNDUP(D10+D10*BEEF_FACTOR,0)</f>
+      <c r="D26" s="49">
+        <f t="shared" ref="D26:M26" si="2">ROUNDUP(D11+D11*BEEF_FACTOR,0)</f>
         <v>157</v>
       </c>
-      <c r="E25" s="62">
+      <c r="E26" s="62">
         <f t="shared" si="2"/>
         <v>188</v>
       </c>
-      <c r="F25" s="49">
+      <c r="F26" s="49">
         <f t="shared" si="2"/>
         <v>625</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G26" s="18">
         <f t="shared" si="2"/>
         <v>2500</v>
       </c>
-      <c r="H25" s="63">
+      <c r="H26" s="63">
         <f t="shared" si="2"/>
         <v>750</v>
       </c>
-      <c r="I25" s="55">
+      <c r="I26" s="55">
         <f t="shared" si="2"/>
         <v>3000</v>
       </c>
-      <c r="J25" s="49">
+      <c r="J26" s="49">
         <f t="shared" si="2"/>
-        <v>625</v>
-      </c>
-      <c r="K25" s="18">
+        <v>0</v>
+      </c>
+      <c r="K26" s="18">
         <f t="shared" si="2"/>
-        <v>3750</v>
-      </c>
-      <c r="L25" s="63">
+        <v>0</v>
+      </c>
+      <c r="L26" s="63">
         <f t="shared" si="2"/>
-        <v>750</v>
-      </c>
-      <c r="M25" s="55">
+        <v>0</v>
+      </c>
+      <c r="M26" s="55">
         <f t="shared" si="2"/>
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="114"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="114"/>
-      <c r="C27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="105" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="101"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B28" s="101"/>
+      <c r="C28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="106"/>
-      <c r="F27" s="105" t="s">
+      <c r="E28" s="105"/>
+      <c r="F28" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="107"/>
-      <c r="H27" s="107"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="105" t="s">
+      <c r="G28" s="106"/>
+      <c r="H28" s="106"/>
+      <c r="I28" s="105"/>
+      <c r="J28" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="K27" s="107"/>
-      <c r="L27" s="107"/>
-      <c r="M27" s="106"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="114"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="108" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="109"/>
-      <c r="H28" s="103" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="104"/>
-      <c r="J28" s="108" t="s">
-        <v>13</v>
-      </c>
-      <c r="K28" s="109"/>
-      <c r="L28" s="103" t="s">
-        <v>14</v>
-      </c>
-      <c r="M28" s="104"/>
+      <c r="K28" s="106"/>
+      <c r="L28" s="106"/>
+      <c r="M28" s="105"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="114"/>
+      <c r="B29" s="101"/>
       <c r="C29" s="3"/>
       <c r="D29" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="107" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="108"/>
+      <c r="H29" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="110"/>
+      <c r="J29" s="107" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="108"/>
+      <c r="L29" s="109" t="s">
+        <v>14</v>
+      </c>
+      <c r="M29" s="110"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B30" s="101"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="57" t="s">
+      <c r="E30" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="56" t="s">
+      <c r="F30" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="G29" s="58" t="s">
+      <c r="G30" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="59" t="s">
+      <c r="H30" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="I29" s="60" t="s">
+      <c r="I30" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="J29" s="56" t="s">
+      <c r="J30" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="K29" s="58" t="s">
+      <c r="K30" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="L29" s="59" t="s">
+      <c r="L30" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="M29" s="60" t="s">
+      <c r="M30" s="60" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="114"/>
-      <c r="C30" s="4" t="s">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B31" s="101"/>
+      <c r="C31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="48">
-        <f t="shared" ref="D30:M30" si="3">ROUNDUP(D15+D15*BEEF_FACTOR,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="50">
+      <c r="D31" s="48">
+        <f t="shared" ref="D31:M31" si="3">ROUNDUP(D16+D16*BEEF_FACTOR,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E31" s="50">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="48">
+        <v>2</v>
+      </c>
+      <c r="F31" s="48">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="G30" s="17">
+      <c r="G31" s="17">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="H30" s="52">
+      <c r="H31" s="52">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="I30" s="53">
+      <c r="I31" s="53">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="J30" s="48">
+      <c r="J31" s="48">
         <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="K30" s="17">
+        <v>0</v>
+      </c>
+      <c r="K31" s="17">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L31" s="52">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="53">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="101"/>
+      <c r="C32" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="48">
+        <f t="shared" ref="D32:M32" si="4">ROUNDUP(D17+D17*BEEF_FACTOR,0)</f>
         <v>5</v>
       </c>
-      <c r="L30" s="52">
-        <f t="shared" si="3"/>
-        <v>3</v>
-      </c>
-      <c r="M30" s="53">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="114"/>
-      <c r="C31" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="48">
-        <f t="shared" ref="D31:M31" si="4">ROUNDUP(D16+D16*BEEF_FACTOR,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="50">
+      <c r="E32" s="50">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="48">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="G31" s="17">
+        <v>6</v>
+      </c>
+      <c r="F32" s="48">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="H31" s="52">
+      <c r="G32" s="17">
         <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="I31" s="53">
+        <v>10</v>
+      </c>
+      <c r="H32" s="52">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="I32" s="53">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="J31" s="48">
+      <c r="J32" s="48">
         <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="K31" s="17">
+        <v>0</v>
+      </c>
+      <c r="K32" s="17">
         <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="L31" s="52">
+        <v>0</v>
+      </c>
+      <c r="L32" s="52">
         <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="M31" s="53">
+        <v>0</v>
+      </c>
+      <c r="M32" s="53">
         <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="115"/>
-      <c r="C32" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="102"/>
+      <c r="C33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="49">
-        <f t="shared" ref="D32:M32" si="5">ROUNDUP(D17+D17*BEEF_FACTOR,0)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="62">
+      <c r="D33" s="49">
+        <f t="shared" ref="D33:M33" si="5">ROUNDUP(D18+D18*BEEF_FACTOR,0)</f>
+        <v>157</v>
+      </c>
+      <c r="E33" s="62">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="49">
+        <v>188</v>
+      </c>
+      <c r="F33" s="49">
         <f t="shared" si="5"/>
         <v>625</v>
       </c>
-      <c r="G32" s="18">
+      <c r="G33" s="18">
         <f t="shared" si="5"/>
         <v>2500</v>
       </c>
-      <c r="H32" s="63">
+      <c r="H33" s="63">
         <f t="shared" si="5"/>
         <v>750</v>
       </c>
-      <c r="I32" s="55">
+      <c r="I33" s="55">
         <f t="shared" si="5"/>
         <v>3000</v>
       </c>
-      <c r="J32" s="49">
+      <c r="J33" s="49">
         <f t="shared" si="5"/>
-        <v>625</v>
-      </c>
-      <c r="K32" s="18">
+        <v>0</v>
+      </c>
+      <c r="K33" s="18">
         <f t="shared" si="5"/>
-        <v>2500</v>
-      </c>
-      <c r="L32" s="63">
+        <v>0</v>
+      </c>
+      <c r="L33" s="63">
         <f t="shared" si="5"/>
-        <v>750</v>
-      </c>
-      <c r="M32" s="55">
+        <v>0</v>
+      </c>
+      <c r="M33" s="55">
         <f t="shared" si="5"/>
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="31">
-    <mergeCell ref="B5:B17"/>
-    <mergeCell ref="B20:B32"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="B6:B18"/>
+    <mergeCell ref="B21:B33"/>
     <mergeCell ref="B2:M2"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
   </mergeCells>
-  <conditionalFormatting sqref="D5:M32">
+  <conditionalFormatting sqref="D6:M33">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3215,7 +3247,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:K6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3228,39 +3260,39 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="D1" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="15">
         <v>92</v>
@@ -3278,7 +3310,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H2" s="15">
         <v>125</v>
@@ -3286,7 +3318,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="15">
         <v>180</v>
@@ -3304,7 +3336,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H3" s="15">
         <v>300</v>
@@ -3312,7 +3344,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B4" s="15">
         <v>476</v>
@@ -3331,7 +3363,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H4" s="15">
         <v>500</v>
@@ -3348,7 +3380,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="15">
         <v>730</v>
@@ -3366,7 +3398,7 @@
         <v>4</v>
       </c>
       <c r="G5" s="15">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="H5" s="15">
         <v>500</v>
@@ -3383,7 +3415,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="15">
         <v>476</v>
@@ -3401,20 +3433,24 @@
         <v>2</v>
       </c>
       <c r="G6" s="15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H6" s="15">
         <v>500</v>
       </c>
-      <c r="I6" s="15">
-        <v>4</v>
-      </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="I6" s="70">
+        <v>8</v>
+      </c>
+      <c r="J6" s="70">
+        <v>16</v>
+      </c>
+      <c r="K6" s="70">
+        <v>3000</v>
+      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="44">
         <v>0.2</v>
@@ -3422,7 +3458,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>21</v>
@@ -3528,15 +3564,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <Project xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">45</Project>
@@ -3545,6 +3572,15 @@
     <Review_x0020_Status xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">Review Completed</Review_x0020_Status>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3565,18 +3601,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C0D350-2871-401C-8D5C-791C478D9E13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312B28CD-EB51-4560-8E58-B9E03DAFD80D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="d4f1fd26-cd3f-48df-8559-6269d85163e3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C0D350-2871-401C-8D5C-791C478D9E13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update capacity planning guidance
</commit_message>
<xml_diff>
--- a/src/Planning/understand-options-tfs-vsts-environments-capacity-guide.xlsx
+++ b/src/Planning/understand-options-tfs-vsts-environments-capacity-guide.xlsx
@@ -1,30 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willy\OneDrive\_repos\Guidance\src\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ken.muse\Source\Repos\ALMRangers Guidance\src\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{2807C006-C69B-4AC9-8D01-14B79F4CDF28}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{B2CD11E7-C4ED-4C84-8FBA-E50379023EA9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBF2B66-D78E-42A8-8FB3-EA1E69F62ECB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="9180" windowWidth="21840" windowHeight="7272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Server Scenarios" sheetId="1" r:id="rId1"/>
-    <sheet name="Hardware Configurations" sheetId="7" r:id="rId2"/>
-    <sheet name="Constants" sheetId="5" state="hidden" r:id="rId3"/>
+    <sheet name="Constants" sheetId="5" state="hidden" r:id="rId2"/>
+    <sheet name="Hardware Configurations" sheetId="7" r:id="rId3"/>
+    <sheet name="Additional Servers" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="Active_Branches">Constants!$B$18</definedName>
     <definedName name="BEEF_FACTOR">'Server Scenarios'!$C$9</definedName>
-    <definedName name="C_NO">Constants!$B$21</definedName>
-    <definedName name="C_YES">Constants!$B$20</definedName>
+    <definedName name="C_NO">Constants!$B$22</definedName>
+    <definedName name="C_YES">Constants!$B$21</definedName>
+    <definedName name="CS_HIGH_CORES">Constants!$C$10</definedName>
+    <definedName name="CS_HIGH_RAM">Constants!$D$10</definedName>
+    <definedName name="CS_HIGH_USERS">Constants!$B$10</definedName>
+    <definedName name="CS_LOW_CORES">Constants!$C$9</definedName>
+    <definedName name="CS_LOW_RAM">Constants!$D$9</definedName>
+    <definedName name="CS_LOW_USERS">Constants!$B$9</definedName>
+    <definedName name="CS_STORAGE_FACTOR">Constants!$B$19</definedName>
+    <definedName name="Current_BranchTip">'Server Scenarios'!$K$7</definedName>
+    <definedName name="Current_Storage">'Server Scenarios'!$F$7</definedName>
     <definedName name="Current_Users">'Server Scenarios'!$C$7</definedName>
     <definedName name="DUAL_CURRENT_OK">'Server Scenarios'!$F$13</definedName>
     <definedName name="DUAL_FUTURE_OK">'Server Scenarios'!$F$14</definedName>
+    <definedName name="Future_BranchTip">'Server Scenarios'!$K$6</definedName>
+    <definedName name="Future_Storage">'Server Scenarios'!$F$6</definedName>
     <definedName name="Future_Users">'Server Scenarios'!$C$6</definedName>
+    <definedName name="GVFS_SCALE_FACTOR">Constants!$B$17</definedName>
     <definedName name="HI_CORE_AT">Constants!$F$5</definedName>
     <definedName name="HI_CORE_DT">Constants!$I$5</definedName>
     <definedName name="HI_DISK_AT">Constants!$H$5</definedName>
@@ -51,6 +65,15 @@
     <definedName name="MEDIUM_RPS">Constants!$B$4</definedName>
     <definedName name="MEDIUM_TPC">Constants!$E$4</definedName>
     <definedName name="MEDIUM_USERS">Constants!$C$4</definedName>
+    <definedName name="PROXY_HIGH_CORES">Constants!$C$15</definedName>
+    <definedName name="PROXY_HIGH_RAM">Constants!$D$15</definedName>
+    <definedName name="PROXY_HIGH_USERS">Constants!$B$15</definedName>
+    <definedName name="PROXY_LOW_CORES">Constants!$C$13</definedName>
+    <definedName name="PROXY_LOW_RAM">Constants!$D$13</definedName>
+    <definedName name="PROXY_LOW_USERS">Constants!$B$13</definedName>
+    <definedName name="PROXY_MEDIUM_CORES">Constants!$C$14</definedName>
+    <definedName name="PROXY_MEDIUM_RAM">Constants!$D$14</definedName>
+    <definedName name="PROXY_MEDIUM_USERS">Constants!$B$14</definedName>
     <definedName name="SCALE_CORE_AT">Constants!$F$6</definedName>
     <definedName name="SCALE_CORE_DT">Constants!$I$6</definedName>
     <definedName name="SCALE_CURRENT_OK">'Server Scenarios'!$I$13</definedName>
@@ -73,14 +96,22 @@
     <definedName name="STANDARD_RPD">Constants!$B$3</definedName>
     <definedName name="STANDARD_TPC">Constants!$E$3</definedName>
     <definedName name="STANDARD_USERS">Constants!$C$3</definedName>
-    <definedName name="VIRTUAL_PERCENTAGE">Constants!$B$19</definedName>
+    <definedName name="VIRTUAL_PERCENTAGE">Constants!$B$20</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="76">
   <si>
     <t>F</t>
   </si>
@@ -315,9 +346,6 @@
     <t>DISK-DT</t>
   </si>
   <si>
-    <t>BETA</t>
-  </si>
-  <si>
     <t>Maximum expected users</t>
   </si>
   <si>
@@ -435,9 +463,6 @@
     </r>
   </si>
   <si>
-    <t>Version 2018.08.03</t>
-  </si>
-  <si>
     <t>Medium-End Configuration</t>
   </si>
   <si>
@@ -465,6 +490,60 @@
       </rPr>
       <t xml:space="preserve"> for up-to-date operating system, hardware, virtualization, and other requirements.</t>
     </r>
+  </si>
+  <si>
+    <t>Version 2019.03.04</t>
+  </si>
+  <si>
+    <t>Code Search Server</t>
+  </si>
+  <si>
+    <t>Standalone Server</t>
+  </si>
+  <si>
+    <t>Code Search Low-End</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Code Search High-End</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Proxy Server</t>
+  </si>
+  <si>
+    <t>Standalone Server With GVFS</t>
+  </si>
+  <si>
+    <t>Search Server Storage</t>
+  </si>
+  <si>
+    <t>Proxy Low-End</t>
+  </si>
+  <si>
+    <t>Proxy Medium-End</t>
+  </si>
+  <si>
+    <t>Proxy High-End</t>
+  </si>
+  <si>
+    <t>Branch Tip Size (GB)</t>
+  </si>
+  <si>
+    <t>Proxy Active Branches</t>
+  </si>
+  <si>
+    <t>GVFS Storage Scale</t>
+  </si>
+  <si>
+    <t>Total Repository (GB)</t>
   </si>
 </sst>
 </file>
@@ -605,13 +684,6 @@
     </font>
     <font>
       <sz val="72"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="72"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -634,6 +706,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -993,19 +1074,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1014,7 +1095,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1032,71 +1113,61 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1135,7 +1206,7 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1144,109 +1215,135 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1266,59 +1363,99 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="4" tint="0.79998168889431442"/>
@@ -1759,334 +1896,365 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I5" sqref="I5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="19"/>
-    <col min="2" max="2" width="64.6640625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="9" style="19" customWidth="1"/>
-    <col min="4" max="4" width="3.33203125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="1.5546875" style="19" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="9" style="19" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" style="19" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="19" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="19"/>
+    <col min="2" max="2" width="64.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="3.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="1.5546875" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" customWidth="1"/>
+    <col min="11" max="11" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
+      <c r="B2" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
-        <v>54</v>
+      <c r="B3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="91" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="95" t="s">
+      <c r="A5" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="96"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="1.65">
-      <c r="A6" s="91"/>
-      <c r="B6" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="67">
-        <v>0</v>
-      </c>
-      <c r="D6" s="21" t="s">
+      <c r="C5" s="67"/>
+      <c r="E5" s="107" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="I5" s="107" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="62"/>
+      <c r="B6" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="59">
+        <v>0</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="64" t="s">
-        <v>50</v>
+      <c r="E6" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="109">
+        <v>0</v>
+      </c>
+      <c r="G6" s="110"/>
+      <c r="I6" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="113"/>
+      <c r="K6" s="59">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="92"/>
-      <c r="B7" s="68" t="s">
+      <c r="A7" s="63"/>
+      <c r="B7" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="69">
-        <v>0</v>
-      </c>
-      <c r="D7" s="21" t="s">
+      <c r="C7" s="61">
+        <v>0</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
+      <c r="E7" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="111">
+        <v>0</v>
+      </c>
+      <c r="G7" s="112"/>
+      <c r="I7" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="114"/>
+      <c r="K7" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="21"/>
+      <c r="A8" s="19"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="22"/>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>0.25</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>55</v>
+      <c r="E9" s="21" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="21"/>
+      <c r="A10" s="19"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="83"/>
-      <c r="E11" s="83"/>
-      <c r="F11" s="83" t="s">
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83" t="s">
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="83"/>
-      <c r="K11" s="84"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="82"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="94"/>
-      <c r="C12" s="85" t="s">
+      <c r="B12" s="65"/>
+      <c r="C12" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="85" t="s">
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
-      <c r="I12" s="85" t="s">
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="85"/>
-      <c r="K12" s="86"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="83"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="87" t="str">
+      <c r="C13" s="72" t="str">
         <f>IF(Current_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87" t="str">
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72" t="str">
         <f>IF(Current_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87" t="str">
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="72" t="str">
         <f>I14</f>
         <v>No</v>
       </c>
-      <c r="J13" s="87"/>
-      <c r="K13" s="88"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="74"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="89" t="str">
+      <c r="C14" s="72" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89" t="str">
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72" t="str">
         <f>IF(Future_Users&gt;HI_USERS,C_NO,C_YES)</f>
         <v>Yes</v>
       </c>
-      <c r="G14" s="89"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89" t="str">
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="72" t="str">
         <f>IF(Future_Users&gt;STANDARD_USERS,C_YES,C_NO)</f>
         <v>No</v>
       </c>
-      <c r="J14" s="89"/>
-      <c r="K14" s="90"/>
+      <c r="J14" s="72"/>
+      <c r="K14" s="74"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="89" t="str">
+      <c r="C15" s="72" t="str">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;1),C_YES,C_NO)</f>
         <v>Yes</v>
       </c>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89" t="str">
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;1),C_YES,C_NO)</f>
         <v>Yes</v>
       </c>
-      <c r="G15" s="89"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89" t="str">
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="72" t="str">
         <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),C_YES,C_NO)</f>
         <v>No</v>
       </c>
-      <c r="J15" s="89"/>
-      <c r="K15" s="90"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="74"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="29" t="str">
+      <c r="C16" s="24" t="str">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
         <v>Low-End</v>
       </c>
-      <c r="D16" s="30" t="str">
+      <c r="D16" s="25" t="str">
         <f>IF(E16="","","-")</f>
         <v>-</v>
       </c>
-      <c r="E16" s="31" t="str">
+      <c r="E16" s="26" t="str">
         <f>IF(C14=C_YES,(IF(Future_Users&gt;LO_USERS,"Standard","Low-End")),"")</f>
         <v>Low-End</v>
       </c>
-      <c r="F16" s="72" t="str">
+      <c r="F16" s="73" t="str">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),"High-End","")</f>
         <v>High-End</v>
       </c>
-      <c r="G16" s="72"/>
-      <c r="H16" s="72"/>
-      <c r="I16" s="72" t="str">
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73" t="str">
         <f>IF((COUNTIF(I13:I14,C_YES)&gt;0),"Scale Unit","")</f>
         <v/>
       </c>
-      <c r="J16" s="72"/>
-      <c r="K16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="76"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="74">
+      <c r="C17" s="70">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
         <v>5</v>
       </c>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74">
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70">
         <f>IF(F13=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74" t="str">
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70" t="str">
         <f>IF(I13=C_YES,SCALE_TPC,"")</f>
         <v/>
       </c>
-      <c r="J17" s="74"/>
+      <c r="J17" s="70"/>
       <c r="K17" s="79"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="80">
+      <c r="C18" s="71">
         <f>IF(C13=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_TPC,LO_TPC)),"")</f>
         <v>5</v>
       </c>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="74">
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="70">
         <f>IF(F14=C_YES,HIGH_TPC,"")</f>
         <v>75</v>
       </c>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="80" t="str">
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="71" t="str">
         <f>IF(I14=C_YES,SCALE_TPC,"")</f>
         <v/>
       </c>
-      <c r="J18" s="80"/>
-      <c r="K18" s="81"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="80"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="82">
+      <c r="C19" s="81">
         <f>IF((COUNTIF(C13:C14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82">
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81">
         <f>IF((COUNTIF(F13:F14,C_YES)&gt;0),1,"")</f>
         <v>1</v>
       </c>
-      <c r="G19" s="82"/>
-      <c r="H19" s="82"/>
-      <c r="I19" s="34" t="str">
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="29" t="str">
         <f>IF(I13=C_YES,ROUNDUP(I20/SCALE_RPS,0),"")</f>
         <v/>
       </c>
-      <c r="J19" s="35" t="str">
+      <c r="J19" s="30" t="str">
         <f>IF(K19&lt;&gt;"","-","")</f>
         <v/>
       </c>
-      <c r="K19" s="36" t="str">
+      <c r="K19" s="31" t="str">
         <f>IF(I14=C_YES,ROUNDUP(K20/SCALE_RPS,0),"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="75">
+      <c r="C20" s="77">
         <f>IF(C13=C_YES,(IF(Current_Users&gt;LO_USERS,Current_Users*STANDARD_FACTOR,Current_Users*LO_FACTOR)),"")</f>
         <v>0</v>
       </c>
-      <c r="D20" s="75" t="str">
+      <c r="D20" s="77" t="str">
         <f>IF(E20&lt;&gt;"","-","")</f>
         <v>-</v>
       </c>
-      <c r="E20" s="75">
+      <c r="E20" s="77">
         <f>IF(C14=C_YES,(IF(Future_Users&gt;LO_USERS,Future_Users*STANDARD_FACTOR,Future_Users*LO_FACTOR)),"")</f>
         <v>0</v>
       </c>
@@ -2094,7 +2262,7 @@
         <f>IF(F13=C_YES,Current_Users*HI_FACTOR,"")</f>
         <v>0</v>
       </c>
-      <c r="G20" s="75" t="str">
+      <c r="G20" s="77" t="str">
         <f>IF(H20&lt;&gt;"","-","")</f>
         <v>-</v>
       </c>
@@ -2102,66 +2270,51 @@
         <f>IF(F14=C_YES,Future_Users*HI_FACTOR,"")</f>
         <v>0</v>
       </c>
-      <c r="I20" s="37" t="str">
+      <c r="I20" s="32" t="str">
         <f>IF(I13=C_YES,Current_Users*SCALE_FACTOR,"")</f>
         <v/>
       </c>
-      <c r="J20" s="38" t="str">
+      <c r="J20" s="16" t="str">
         <f>IF(K20&lt;&gt;"","-","")</f>
         <v/>
       </c>
-      <c r="K20" s="39" t="str">
+      <c r="K20" s="33" t="str">
         <f>IF(I13=C_YES,Future_Users*HI_FACTOR,"")</f>
         <v/>
       </c>
     </row>
     <row r="21" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
       <c r="F21" s="78"/>
-      <c r="G21" s="76"/>
+      <c r="G21" s="78"/>
       <c r="H21" s="78"/>
-      <c r="I21" s="41" t="str">
+      <c r="I21" s="35" t="str">
         <f>IF(I13=C_YES,I20/I19,"")</f>
         <v/>
       </c>
-      <c r="J21" s="42" t="str">
+      <c r="J21" s="17" t="str">
         <f>IF(K21&lt;&gt;"","-","")</f>
         <v/>
       </c>
-      <c r="K21" s="43" t="str">
+      <c r="K21" s="36" t="str">
         <f>IF(I14=C_YES,K20/K19,"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:11" ht="91.8" x14ac:dyDescent="1.65">
-      <c r="B24" s="65"/>
+      <c r="B24" s="57"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
+  <mergeCells count="39">
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I5:K5"/>
     <mergeCell ref="B2:K2"/>
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="F17:H17"/>
@@ -2178,27 +2331,46 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="I12:K12"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
   </mergeCells>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="17" priority="13">
       <formula>$C$6&gt;=$C$7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8 D10">
-    <cfRule type="expression" dxfId="6" priority="12">
+    <cfRule type="expression" dxfId="16" priority="12">
       <formula>$C$7&lt;=$C$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:C15 F13:F16 I13:I16">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>$C$9&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2238,12 +2410,369 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.5546875" customWidth="1"/>
+    <col min="2" max="3" width="11" style="14" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="14">
+        <v>92</v>
+      </c>
+      <c r="C2" s="14">
+        <v>250</v>
+      </c>
+      <c r="D2">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E2" s="14">
+        <v>5</v>
+      </c>
+      <c r="F2" s="14">
+        <v>2</v>
+      </c>
+      <c r="G2" s="14">
+        <v>4</v>
+      </c>
+      <c r="H2" s="14">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="14">
+        <v>180</v>
+      </c>
+      <c r="C3" s="14">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E3" s="14">
+        <v>10</v>
+      </c>
+      <c r="F3" s="14">
+        <v>2</v>
+      </c>
+      <c r="G3" s="14">
+        <v>8</v>
+      </c>
+      <c r="H3" s="14">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="14">
+        <v>476</v>
+      </c>
+      <c r="C4" s="14">
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>0.21249999999999999</v>
+      </c>
+      <c r="E4" s="14">
+        <f>SCALE_TPC</f>
+        <v>75</v>
+      </c>
+      <c r="F4" s="14">
+        <v>2</v>
+      </c>
+      <c r="G4" s="14">
+        <v>8</v>
+      </c>
+      <c r="H4" s="14">
+        <v>500</v>
+      </c>
+      <c r="I4" s="14">
+        <v>4</v>
+      </c>
+      <c r="J4" s="14">
+        <v>8</v>
+      </c>
+      <c r="K4" s="14">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="14">
+        <v>730</v>
+      </c>
+      <c r="C5" s="14">
+        <v>3600</v>
+      </c>
+      <c r="D5">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="E5" s="14">
+        <v>75</v>
+      </c>
+      <c r="F5" s="14">
+        <v>4</v>
+      </c>
+      <c r="G5" s="14">
+        <v>16</v>
+      </c>
+      <c r="H5" s="14">
+        <v>500</v>
+      </c>
+      <c r="I5" s="14">
+        <v>8</v>
+      </c>
+      <c r="J5" s="14">
+        <v>16</v>
+      </c>
+      <c r="K5" s="14">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="14">
+        <v>476</v>
+      </c>
+      <c r="C6" s="14">
+        <v>2200</v>
+      </c>
+      <c r="D6">
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="E6" s="14">
+        <v>75</v>
+      </c>
+      <c r="F6" s="14">
+        <v>2</v>
+      </c>
+      <c r="G6" s="14">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14">
+        <v>500</v>
+      </c>
+      <c r="I6" s="14">
+        <v>8</v>
+      </c>
+      <c r="J6" s="14">
+        <v>16</v>
+      </c>
+      <c r="K6" s="14">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="105" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="14">
+        <v>500</v>
+      </c>
+      <c r="C9" s="14">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="14">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="105" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="14">
+        <v>450</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="14">
+        <v>2200</v>
+      </c>
+      <c r="C14" s="14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="14">
+        <v>3600</v>
+      </c>
+      <c r="C15" s="14">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="106">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="37">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:M33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2259,940 +2788,930 @@
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="103" t="str">
+      <c r="B2" s="72" t="str">
         <f>'Server Scenarios'!B2:K2</f>
-        <v>Version 2018.08.03</v>
-      </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
+        <v>Version 2019.03.04</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="118" t="s">
-        <v>56</v>
+      <c r="B3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="97" t="s">
-        <v>52</v>
+      <c r="B6" s="98" t="s">
+        <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="111" t="s">
+      <c r="D6" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="112"/>
-      <c r="F6" s="111" t="s">
+      <c r="E6" s="85"/>
+      <c r="F6" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="113"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="111" t="s">
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="113"/>
-      <c r="L6" s="113"/>
-      <c r="M6" s="112"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="85"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="98"/>
+      <c r="B7" s="99"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F7" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="115"/>
-      <c r="H7" s="116" t="s">
+      <c r="G7" s="88"/>
+      <c r="H7" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="115"/>
-      <c r="J7" s="114" t="s">
+      <c r="I7" s="88"/>
+      <c r="J7" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="115"/>
-      <c r="L7" s="116" t="s">
+      <c r="K7" s="88"/>
+      <c r="L7" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="117"/>
+      <c r="M7" s="90"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="98"/>
+      <c r="B8" s="99"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="98"/>
+      <c r="B9" s="99"/>
       <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="41">
         <f>IF(SINGLE_CURRENT_OK=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_CORE_AT,LO_CORE_AT)),0)</f>
-        <v>1</v>
-      </c>
-      <c r="E9" s="50">
+        <v>2</v>
+      </c>
+      <c r="E9" s="43">
         <f>IFD9+D9*VIRTUAL_PERCENTAGE</f>
-        <v>0.2</v>
-      </c>
-      <c r="F9" s="48">
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="41">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_CORE_AT,MEDIUM_CORE_AT)),0)</f>
         <v>2</v>
       </c>
-      <c r="G9" s="51">
+      <c r="G9" s="44">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_CORE_DT,MEDIUM_CORE_DT)),0)</f>
         <v>4</v>
       </c>
-      <c r="H9" s="52">
+      <c r="H9" s="45">
         <f>F9+F9*VIRTUAL_PERCENTAGE</f>
         <v>2.4</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="16">
         <f>IF(G9&lt;&gt;"",ROUNDUP(G9+G9*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>5</v>
       </c>
-      <c r="J9" s="48">
+      <c r="J9" s="41">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_CORE_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="51">
+      <c r="K9" s="44">
         <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;SCALE_USERS,SCALE_CORE_DT,SCALE_CORE_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L9" s="52">
+      <c r="L9" s="45">
         <f>J9+J9*VIRTUAL_PERCENTAGE</f>
         <v>0</v>
       </c>
-      <c r="M9" s="53">
+      <c r="M9" s="46">
         <f>IF(K9&lt;&gt;"",ROUNDUP(K9+K9*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="98"/>
+      <c r="B10" s="99"/>
       <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="41">
         <f>IF(SINGLE_CURRENT_OK=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_RAM_AT,LO_RAM_AT)),0)</f>
         <v>4</v>
       </c>
-      <c r="E10" s="50">
+      <c r="E10" s="43">
         <f>D10+D10*VIRTUAL_PERCENTAGE</f>
         <v>4.8</v>
       </c>
-      <c r="F10" s="48">
+      <c r="F10" s="41">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_RAM_AT,MEDIUM_RAM_AT)),0)</f>
         <v>8</v>
       </c>
-      <c r="G10" s="51">
+      <c r="G10" s="44">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_RAM_DT,MEDIUM_RAM_DT)),0)</f>
         <v>8</v>
       </c>
-      <c r="H10" s="52">
+      <c r="H10" s="45">
         <f>F10+F10*VIRTUAL_PERCENTAGE</f>
         <v>9.6</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="16">
         <f>IF(G10&lt;&gt;"",ROUNDUP(G10+G10*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>10</v>
       </c>
-      <c r="J10" s="48">
+      <c r="J10" s="41">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_RAM_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K10" s="51">
+      <c r="K10" s="44">
         <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;SCALE_USERS,SCALE_RAM_DT,SCALE_RAM_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L10" s="52">
+      <c r="L10" s="45">
         <f>J10+J10*VIRTUAL_PERCENTAGE</f>
         <v>0</v>
       </c>
-      <c r="M10" s="53">
+      <c r="M10" s="46">
         <f>IF(K10&lt;&gt;"",ROUNDUP(K10+K10*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="98"/>
+      <c r="B11" s="99"/>
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="42">
         <f>IF(SINGLE_CURRENT_OK=C_YES,(IF(Current_Users&gt;LO_USERS,STANDARD_DISK_AT,LO_DISK_AT)),0)</f>
         <v>125</v>
       </c>
-      <c r="E11" s="62">
+      <c r="E11" s="55">
         <f>D11+D11*VIRTUAL_PERCENTAGE</f>
         <v>150</v>
       </c>
-      <c r="F11" s="49">
+      <c r="F11" s="42">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_DISK_AT,MEDIUM_DISK_AT)),0)</f>
         <v>500</v>
       </c>
-      <c r="G11" s="54">
+      <c r="G11" s="47">
         <f>IF(DUAL_CURRENT_OK=C_YES,(IF(Current_Users&gt;MEDIUM_USERS,HI_DISK_DT,MEDIUM_DISK_DT)),0)</f>
         <v>2000</v>
       </c>
-      <c r="H11" s="63">
+      <c r="H11" s="56">
         <f>F11+F11*VIRTUAL_PERCENTAGE</f>
         <v>600</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="17">
         <f>IF(G11&lt;&gt;"",ROUNDUP(G11+G11*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>2400</v>
       </c>
-      <c r="J11" s="49">
+      <c r="J11" s="42">
         <f>IF(SCALE_CURRENT_OK=C_YES,SCALE_DISK_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="54">
+      <c r="K11" s="47">
         <f>IF(SCALE_CURRENT_OK=C_YES,(IF(Current_Users&gt;SCALE_USERS,SCALE_DISK_DT,SCALE_DISK_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="63">
+      <c r="L11" s="56">
         <f>J11+J11*VIRTUAL_PERCENTAGE</f>
         <v>0</v>
       </c>
-      <c r="M11" s="55">
+      <c r="M11" s="48">
         <f>IF(K11&lt;&gt;"",ROUNDUP(K11+K11*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="98"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="B12" s="99"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="98"/>
-      <c r="C13" s="45" t="s">
+      <c r="B13" s="99"/>
+      <c r="C13" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="104" t="s">
+      <c r="D13" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="105"/>
-      <c r="F13" s="104" t="s">
+      <c r="E13" s="94"/>
+      <c r="F13" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="106"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="106"/>
-      <c r="J13" s="104" t="s">
+      <c r="G13" s="95"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="95"/>
+      <c r="J13" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="106"/>
-      <c r="L13" s="106"/>
-      <c r="M13" s="105"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="94"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="98"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="56" t="s">
+      <c r="B14" s="99"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="107" t="s">
+      <c r="F14" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="108"/>
-      <c r="H14" s="109" t="s">
+      <c r="G14" s="97"/>
+      <c r="H14" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="108"/>
-      <c r="J14" s="107" t="s">
+      <c r="I14" s="97"/>
+      <c r="J14" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="108"/>
-      <c r="L14" s="109" t="s">
+      <c r="K14" s="97"/>
+      <c r="L14" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="M14" s="110"/>
+      <c r="M14" s="92"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="98"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="56" t="s">
+      <c r="B15" s="99"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="58" t="s">
+      <c r="G15" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="H15" s="59" t="s">
+      <c r="H15" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="58" t="s">
+      <c r="I15" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="56" t="s">
+      <c r="J15" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="58" t="s">
+      <c r="K15" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="59" t="s">
+      <c r="L15" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="60" t="s">
+      <c r="M15" s="53" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="98"/>
-      <c r="C16" s="46" t="s">
+      <c r="B16" s="99"/>
+      <c r="C16" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="41">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_CORE_AT,LO_CORE_AT)),0)</f>
-        <v>1</v>
-      </c>
-      <c r="E16" s="50">
+        <v>2</v>
+      </c>
+      <c r="E16" s="43">
         <f>D16+D16*VIRTUAL_PERCENTAGE</f>
-        <v>1.2</v>
-      </c>
-      <c r="F16" s="48">
+        <v>2.4</v>
+      </c>
+      <c r="F16" s="41">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_CORE_AT,MEDIUM_CORE_AT)),0)</f>
         <v>2</v>
       </c>
-      <c r="G16" s="51">
+      <c r="G16" s="44">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_CORE_DT,MEDIUM_CORE_DT)),0)</f>
         <v>4</v>
       </c>
-      <c r="H16" s="52">
+      <c r="H16" s="45">
         <f>F16+F16*VIRTUAL_PERCENTAGE</f>
         <v>2.4</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="16">
         <f>IF(G16&lt;&gt;"",ROUNDUP(G16+G16*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>5</v>
       </c>
-      <c r="J16" s="48">
+      <c r="J16" s="41">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_CORE_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="51">
+      <c r="K16" s="44">
         <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;SCALE_USERS,SCALE_CORE_DT,SCALE_CORE_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L16" s="52">
+      <c r="L16" s="45">
         <f>J16+J16*VIRTUAL_PERCENTAGE</f>
         <v>0</v>
       </c>
-      <c r="M16" s="53">
+      <c r="M16" s="46">
         <f>IF(K16&lt;&gt;"",ROUNDUP(K16+K16*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="98"/>
-      <c r="C17" s="46" t="s">
+      <c r="B17" s="99"/>
+      <c r="C17" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="41">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_RAM_AT,LO_RAM_AT)),0)</f>
         <v>4</v>
       </c>
-      <c r="E17" s="50">
+      <c r="E17" s="43">
         <f>D17+D17*VIRTUAL_PERCENTAGE</f>
         <v>4.8</v>
       </c>
-      <c r="F17" s="48">
+      <c r="F17" s="41">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_RAM_AT,MEDIUM_RAM_AT)),0)</f>
         <v>8</v>
       </c>
-      <c r="G17" s="51">
+      <c r="G17" s="44">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_RAM_DT,MEDIUM_RAM_DT)),0)</f>
         <v>8</v>
       </c>
-      <c r="H17" s="52">
+      <c r="H17" s="45">
         <f>F17+F17*VIRTUAL_PERCENTAGE</f>
         <v>9.6</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="16">
         <f>IF(G17&lt;&gt;"",ROUNDUP(G17+G17*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>10</v>
       </c>
-      <c r="J17" s="48">
+      <c r="J17" s="41">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_RAM_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="51">
+      <c r="K17" s="44">
         <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;SCALE_USERS,SCALE_RAM_DT,SCALE_RAM_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L17" s="52">
+      <c r="L17" s="45">
         <f>J17+J17*VIRTUAL_PERCENTAGE</f>
         <v>0</v>
       </c>
-      <c r="M17" s="53">
+      <c r="M17" s="46">
         <f>IF(K17&lt;&gt;"",ROUNDUP(K17+K17*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="99"/>
-      <c r="C18" s="47" t="s">
+      <c r="B18" s="100"/>
+      <c r="C18" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="42">
         <f>IF(SINGLE_FUTURE_OK=C_YES,(IF(Future_Users&gt;LO_USERS,STANDARD_DISK_AT,LO_DISK_AT)),0)</f>
         <v>125</v>
       </c>
-      <c r="E18" s="62">
+      <c r="E18" s="55">
         <f>D18+D18*VIRTUAL_PERCENTAGE</f>
         <v>150</v>
       </c>
-      <c r="F18" s="49">
+      <c r="F18" s="42">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,MEDIUM_DISK_AT,HI_DISK_AT)),0)</f>
         <v>500</v>
       </c>
-      <c r="G18" s="54">
+      <c r="G18" s="47">
         <f>IF(DUAL_FUTURE_OK=C_YES,(IF(Future_Users&gt;MEDIUM_USERS,HI_DISK_DT,MEDIUM_DISK_DT)),0)</f>
         <v>2000</v>
       </c>
-      <c r="H18" s="63">
+      <c r="H18" s="56">
         <f>F18+F18*VIRTUAL_PERCENTAGE</f>
         <v>600</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="17">
         <f>IF(G18&lt;&gt;"",ROUNDUP(G18+G18*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>2400</v>
       </c>
-      <c r="J18" s="49">
+      <c r="J18" s="42">
         <f>IF(SCALE_FUTURE_OK=C_YES,SCALE_DISK_AT,0)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="54">
+      <c r="K18" s="47">
         <f>IF(SCALE_FUTURE_OK=C_YES,(IF(Future_Users&gt;SCALE_USERS,SCALE_DISK_DT,SCALE_DISK_DT)),0)</f>
         <v>0</v>
       </c>
-      <c r="L18" s="63">
+      <c r="L18" s="56">
         <f>J18+J18*VIRTUAL_PERCENTAGE</f>
         <v>0</v>
       </c>
-      <c r="M18" s="55">
+      <c r="M18" s="48">
         <f>IF(K18&lt;&gt;"",ROUNDUP(K18+K18*VIRTUAL_PERCENTAGE,0),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="100" t="s">
-        <v>53</v>
+      <c r="B21" s="101" t="s">
+        <v>52</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="104" t="s">
+      <c r="D21" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="105"/>
-      <c r="F21" s="104" t="s">
+      <c r="E21" s="94"/>
+      <c r="F21" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="105"/>
-      <c r="J21" s="104" t="s">
+      <c r="G21" s="95"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="94"/>
+      <c r="J21" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="K21" s="106"/>
-      <c r="L21" s="106"/>
-      <c r="M21" s="105"/>
+      <c r="K21" s="95"/>
+      <c r="L21" s="95"/>
+      <c r="M21" s="94"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="101"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="56" t="s">
+      <c r="D22" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="F22" s="107" t="s">
+      <c r="F22" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="108"/>
-      <c r="H22" s="109" t="s">
+      <c r="G22" s="97"/>
+      <c r="H22" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="110"/>
-      <c r="J22" s="107" t="s">
+      <c r="I22" s="92"/>
+      <c r="J22" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="K22" s="108"/>
-      <c r="L22" s="109" t="s">
+      <c r="K22" s="97"/>
+      <c r="L22" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="M22" s="110"/>
+      <c r="M22" s="92"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="101"/>
+      <c r="B23" s="102"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="56" t="s">
+      <c r="D23" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="58" t="s">
+      <c r="G23" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H23" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="60" t="s">
+      <c r="I23" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="56" t="s">
+      <c r="J23" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="58" t="s">
+      <c r="K23" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="L23" s="59" t="s">
+      <c r="L23" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="M23" s="60" t="s">
+      <c r="M23" s="53" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="101"/>
+      <c r="B24" s="102"/>
       <c r="C24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="48">
+      <c r="D24" s="41">
         <f t="shared" ref="D24:M24" si="0">ROUNDUP(D9+D9*BEEF_FACTOR,0)</f>
-        <v>2</v>
-      </c>
-      <c r="E24" s="50">
+        <v>3</v>
+      </c>
+      <c r="E24" s="43">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F24" s="48">
+      <c r="F24" s="41">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G24" s="17">
+      <c r="G24" s="16">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="H24" s="52">
+      <c r="H24" s="45">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I24" s="53">
+      <c r="I24" s="46">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J24" s="48">
+      <c r="J24" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K24" s="17">
+      <c r="K24" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L24" s="52">
+      <c r="L24" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M24" s="53">
+      <c r="M24" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="101"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="48">
+      <c r="D25" s="41">
         <f t="shared" ref="D25:M25" si="1">ROUNDUP(D10+D10*BEEF_FACTOR,0)</f>
         <v>5</v>
       </c>
-      <c r="E25" s="50">
+      <c r="E25" s="43">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="F25" s="48">
+      <c r="F25" s="41">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="16">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H25" s="52">
+      <c r="H25" s="45">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I25" s="53">
+      <c r="I25" s="46">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="J25" s="48">
+      <c r="J25" s="41">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K25" s="17">
+      <c r="K25" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L25" s="52">
+      <c r="L25" s="45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M25" s="53">
+      <c r="M25" s="46">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="101"/>
+      <c r="B26" s="102"/>
       <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="49">
+      <c r="D26" s="42">
         <f t="shared" ref="D26:M26" si="2">ROUNDUP(D11+D11*BEEF_FACTOR,0)</f>
         <v>157</v>
       </c>
-      <c r="E26" s="62">
+      <c r="E26" s="55">
         <f t="shared" si="2"/>
         <v>188</v>
       </c>
-      <c r="F26" s="49">
+      <c r="F26" s="42">
         <f t="shared" si="2"/>
         <v>625</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="17">
         <f t="shared" si="2"/>
         <v>2500</v>
       </c>
-      <c r="H26" s="63">
+      <c r="H26" s="56">
         <f t="shared" si="2"/>
         <v>750</v>
       </c>
-      <c r="I26" s="55">
+      <c r="I26" s="48">
         <f t="shared" si="2"/>
         <v>3000</v>
       </c>
-      <c r="J26" s="49">
+      <c r="J26" s="42">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K26" s="18">
+      <c r="K26" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L26" s="63">
+      <c r="L26" s="56">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M26" s="55">
+      <c r="M26" s="48">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="101"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
+      <c r="B27" s="102"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="101"/>
+      <c r="B28" s="102"/>
       <c r="C28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="104" t="s">
+      <c r="D28" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="105"/>
-      <c r="F28" s="104" t="s">
+      <c r="E28" s="94"/>
+      <c r="F28" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="106"/>
-      <c r="H28" s="106"/>
-      <c r="I28" s="105"/>
-      <c r="J28" s="104" t="s">
+      <c r="G28" s="95"/>
+      <c r="H28" s="95"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="K28" s="106"/>
-      <c r="L28" s="106"/>
-      <c r="M28" s="105"/>
+      <c r="K28" s="95"/>
+      <c r="L28" s="95"/>
+      <c r="M28" s="94"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="101"/>
+      <c r="B29" s="102"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="56" t="s">
+      <c r="D29" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="57" t="s">
+      <c r="E29" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="107" t="s">
+      <c r="F29" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="108"/>
-      <c r="H29" s="109" t="s">
+      <c r="G29" s="97"/>
+      <c r="H29" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="I29" s="110"/>
-      <c r="J29" s="107" t="s">
+      <c r="I29" s="92"/>
+      <c r="J29" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="K29" s="108"/>
-      <c r="L29" s="109" t="s">
+      <c r="K29" s="97"/>
+      <c r="L29" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="M29" s="110"/>
+      <c r="M29" s="92"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="101"/>
+      <c r="B30" s="102"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="57" t="s">
+      <c r="E30" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="56" t="s">
+      <c r="F30" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G30" s="58" t="s">
+      <c r="G30" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="H30" s="59" t="s">
+      <c r="H30" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="I30" s="60" t="s">
+      <c r="I30" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="56" t="s">
+      <c r="J30" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="K30" s="58" t="s">
+      <c r="K30" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="L30" s="59" t="s">
+      <c r="L30" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="M30" s="60" t="s">
+      <c r="M30" s="53" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="101"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="48">
+      <c r="D31" s="41">
         <f t="shared" ref="D31:M31" si="3">ROUNDUP(D16+D16*BEEF_FACTOR,0)</f>
-        <v>2</v>
-      </c>
-      <c r="E31" s="50">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="F31" s="48">
+        <v>3</v>
+      </c>
+      <c r="E31" s="43">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="G31" s="17">
+      <c r="F31" s="41">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G31" s="16">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="H31" s="52">
+      <c r="H31" s="45">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="I31" s="53">
+      <c r="I31" s="46">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="J31" s="48">
+      <c r="J31" s="41">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K31" s="17">
+      <c r="K31" s="16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L31" s="52">
+      <c r="L31" s="45">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M31" s="53">
+      <c r="M31" s="46">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="101"/>
+      <c r="B32" s="102"/>
       <c r="C32" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="48">
+      <c r="D32" s="41">
         <f t="shared" ref="D32:M32" si="4">ROUNDUP(D17+D17*BEEF_FACTOR,0)</f>
         <v>5</v>
       </c>
-      <c r="E32" s="50">
+      <c r="E32" s="43">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="F32" s="48">
+      <c r="F32" s="41">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G32" s="16">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="H32" s="52">
+      <c r="H32" s="45">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="I32" s="53">
+      <c r="I32" s="46">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="J32" s="48">
+      <c r="J32" s="41">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K32" s="17">
+      <c r="K32" s="16">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L32" s="52">
+      <c r="L32" s="45">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M32" s="53">
+      <c r="M32" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="102"/>
+      <c r="B33" s="103"/>
       <c r="C33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="49">
+      <c r="D33" s="42">
         <f t="shared" ref="D33:M33" si="5">ROUNDUP(D18+D18*BEEF_FACTOR,0)</f>
         <v>157</v>
       </c>
-      <c r="E33" s="62">
+      <c r="E33" s="55">
         <f t="shared" si="5"/>
         <v>188</v>
       </c>
-      <c r="F33" s="49">
+      <c r="F33" s="42">
         <f t="shared" si="5"/>
         <v>625</v>
       </c>
-      <c r="G33" s="18">
+      <c r="G33" s="17">
         <f t="shared" si="5"/>
         <v>2500</v>
       </c>
-      <c r="H33" s="63">
+      <c r="H33" s="56">
         <f t="shared" si="5"/>
         <v>750</v>
       </c>
-      <c r="I33" s="55">
+      <c r="I33" s="48">
         <f t="shared" si="5"/>
         <v>3000</v>
       </c>
-      <c r="J33" s="49">
+      <c r="J33" s="42">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K33" s="18">
+      <c r="K33" s="17">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L33" s="63">
+      <c r="L33" s="56">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="M33" s="55">
+      <c r="M33" s="48">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3200,21 +3719,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="31">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L14:M14"/>
     <mergeCell ref="B6:B18"/>
     <mergeCell ref="B21:B33"/>
     <mergeCell ref="B2:M2"/>
@@ -3231,9 +3735,24 @@
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:M33">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3242,239 +3761,464 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K21"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B24151-BCDB-4D54-B778-984CD476EECE}">
+  <dimension ref="B1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" customWidth="1"/>
-    <col min="2" max="3" width="11" style="15" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="15"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="67.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="15">
-        <v>92</v>
-      </c>
-      <c r="C2" s="15">
-        <v>250</v>
-      </c>
-      <c r="D2">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="E2" s="15">
-        <v>5</v>
-      </c>
-      <c r="F2" s="15">
+    <row r="1" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="72" t="str">
+        <f>'Server Scenarios'!B2:K2</f>
+        <v>Version 2019.03.04</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="104" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="85"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="99"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="99"/>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="41">
+        <f>IF(Current_Users&gt;CS_LOW_USERS,CS_HIGH_CORES,CS_LOW_CORES)</f>
+        <v>2</v>
+      </c>
+      <c r="E8" s="43">
+        <f>D8*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="99"/>
+      <c r="C9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="41">
+        <f>IF(Current_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
+        <v>8</v>
+      </c>
+      <c r="E9" s="43">
+        <f>D9*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="99"/>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="42">
+        <f>Current_Storage*CS_STORAGE_FACTOR</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="55">
+        <f>D10*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="99"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="99"/>
+      <c r="C12" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="85"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="99"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="99"/>
+      <c r="C14" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="41">
+        <f>IF(Future_Users&gt;CS_LOW_USERS,CS_HIGH_CORES,CS_LOW_CORES)</f>
+        <v>2</v>
+      </c>
+      <c r="E14" s="43">
+        <f>D14*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="99"/>
+      <c r="C15" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="41">
+        <f>IF(Future_Users&gt;CS_LOW_USERS,CS_HIGH_RAM,CS_LOW_RAM)</f>
+        <v>8</v>
+      </c>
+      <c r="E15" s="43">
+        <f>D15*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="100"/>
+      <c r="C16" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="42">
+        <f>Future_Storage*CS_STORAGE_FACTOR</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="55">
+        <f>D16*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="104" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="85"/>
+      <c r="F18" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="85"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="99"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="99"/>
+      <c r="C20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="41">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
         <v>1</v>
       </c>
-      <c r="G2" s="15">
-        <v>4</v>
-      </c>
-      <c r="H2" s="15">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="15">
-        <v>180</v>
-      </c>
-      <c r="C3" s="15">
-        <v>500</v>
-      </c>
-      <c r="D3">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="E3" s="15">
-        <v>10</v>
-      </c>
-      <c r="F3" s="15">
+      <c r="E20" s="43">
+        <f>D20*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>1.2</v>
+      </c>
+      <c r="F20" s="41">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="43">
+        <f>F20*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="99"/>
+      <c r="C21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="41">
+        <f>IF(Current_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Current_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
         <v>2</v>
       </c>
-      <c r="G3" s="15">
-        <v>8</v>
-      </c>
-      <c r="H3" s="15">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="15">
-        <v>476</v>
-      </c>
-      <c r="C4" s="15">
-        <v>2200</v>
-      </c>
-      <c r="D4">
-        <v>0.21249999999999999</v>
-      </c>
-      <c r="E4" s="15">
-        <f>SCALE_TPC</f>
-        <v>75</v>
-      </c>
-      <c r="F4" s="15">
+      <c r="E21" s="43">
+        <f>D21*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>2.4</v>
+      </c>
+      <c r="F21" s="41">
+        <f>D21+(Current_BranchTip)</f>
         <v>2</v>
       </c>
-      <c r="G4" s="15">
-        <v>8</v>
-      </c>
-      <c r="H4" s="15">
-        <v>500</v>
-      </c>
-      <c r="I4" s="15">
-        <v>4</v>
-      </c>
-      <c r="J4" s="15">
-        <v>8</v>
-      </c>
-      <c r="K4" s="15">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="15">
-        <v>730</v>
-      </c>
-      <c r="C5" s="15">
-        <v>3600</v>
-      </c>
-      <c r="D5">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="E5" s="15">
-        <v>75</v>
-      </c>
-      <c r="F5" s="15">
-        <v>4</v>
-      </c>
-      <c r="G5" s="15">
-        <v>16</v>
-      </c>
-      <c r="H5" s="15">
-        <v>500</v>
-      </c>
-      <c r="I5" s="15">
-        <v>8</v>
-      </c>
-      <c r="J5" s="15">
-        <v>16</v>
-      </c>
-      <c r="K5" s="15">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="15">
-        <v>476</v>
-      </c>
-      <c r="C6" s="15">
-        <v>2200</v>
-      </c>
-      <c r="D6">
-        <v>0.26250000000000001</v>
-      </c>
-      <c r="E6" s="15">
-        <v>75</v>
-      </c>
-      <c r="F6" s="15">
+      <c r="G21" s="43">
+        <f>F21*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="99"/>
+      <c r="C22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="42">
+        <f>Current_BranchTip*Active_Branches</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="55">
+        <f>D22*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="42">
+        <f>D22+(Current_Storage*GVFS_SCALE_FACTOR)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="55">
+        <f>F22*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="99"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="99"/>
+      <c r="C24" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="85"/>
+      <c r="F24" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="85"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="99"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="99"/>
+      <c r="C26" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="41">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="43">
+        <f>D26*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>1.2</v>
+      </c>
+      <c r="F26" s="41">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_CORES, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_CORES,PROXY_MEDIUM_CORES))</f>
+        <v>1</v>
+      </c>
+      <c r="G26" s="43">
+        <f>F26*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="99"/>
+      <c r="C27" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="41">
+        <f>IF(Future_Users&lt;=PROXY_LOW_USERS,PROXY_LOW_RAM, IF(Future_Users&gt;PROXY_MEDIUM_USERS,PROXY_HIGH_RAM,PROXY_MEDIUM_RAM))</f>
         <v>2</v>
       </c>
-      <c r="G6" s="15">
-        <v>8</v>
-      </c>
-      <c r="H6" s="15">
-        <v>500</v>
-      </c>
-      <c r="I6" s="70">
-        <v>8</v>
-      </c>
-      <c r="J6" s="70">
-        <v>16</v>
-      </c>
-      <c r="K6" s="70">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="44">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="15" t="s">
-        <v>22</v>
+      <c r="E27" s="43">
+        <f>D27*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>2.4</v>
+      </c>
+      <c r="F27" s="41">
+        <f>D27+Future_BranchTip</f>
+        <v>2</v>
+      </c>
+      <c r="G27" s="43">
+        <f>F27*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="100"/>
+      <c r="C28" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="42">
+        <f>Future_BranchTip*Active_Branches</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="55">
+        <f>D28*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="42">
+        <f>D28+(Future_Storage*GVFS_SCALE_FACTOR)</f>
+        <v>0</v>
+      </c>
+      <c r="G28" s="55">
+        <f>F28*(1+VIRTUAL_PERCENTAGE)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="9">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B18:B28"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B6:B16"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D12:E12"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D6:E17">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:E28 D19:E23">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:E18">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24:E24">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19:G19 G20:G22">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:G18">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25:G25 G26:G28">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26:F28">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24:G24">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20:F22">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Project xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">45</Project>
+    <Priority xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">2 - Cheat sheet / posters (high)</Priority>
+    <Notes0 xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3" xsi:nil="true"/>
+    <Review_x0020_Status xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">Review Completed</Review_x0020_Status>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CC8AB984F9AFA14087035BD77D90A626" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="587f6fb58f55cab20468d5767da9b76d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="d4f1fd26-cd3f-48df-8559-6269d85163e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d45bfae41b7a5cd5eac582b346e06dc" ns1:_="">
     <xsd:import namespace="d4f1fd26-cd3f-48df-8559-6269d85163e3"/>
@@ -3563,27 +4307,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Project xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">45</Project>
-    <Priority xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">2 - Cheat sheet / posters (high)</Priority>
-    <Notes0 xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3" xsi:nil="true"/>
-    <Review_x0020_Status xmlns="d4f1fd26-cd3f-48df-8559-6269d85163e3">Review Completed</Review_x0020_Status>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C0D350-2871-401C-8D5C-791C478D9E13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312B28CD-EB51-4560-8E58-B9E03DAFD80D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d4f1fd26-cd3f-48df-8559-6269d85163e3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E2C743B-52BB-4B93-BC7B-301A591373EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3598,21 +4339,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{312B28CD-EB51-4560-8E58-B9E03DAFD80D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d4f1fd26-cd3f-48df-8559-6269d85163e3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C0D350-2871-401C-8D5C-791C478D9E13}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>